<commit_message>
Pilot 1 - User 3.
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="23955" windowHeight="12840" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="23955" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="target" sheetId="1" r:id="rId1"/>
@@ -935,33 +935,33 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.6</c:v>
+                  <c:v>0.53</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.42666666666666664</c:v>
+                  <c:v>0.32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="48413312"/>
-        <c:axId val="48423296"/>
+        <c:axId val="115739648"/>
+        <c:axId val="115741440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48413312"/>
+        <c:axId val="115739648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48423296"/>
+        <c:crossAx val="115741440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48423296"/>
+        <c:axId val="115741440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -971,7 +971,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48413312"/>
+        <c:crossAx val="115739648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -980,7 +980,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1028,42 +1028,42 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.46666666666666662</c:v>
+                  <c:v>0.42499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.6</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.46666666666666662</c:v>
+                  <c:v>0.375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.53333333333333333</c:v>
+                  <c:v>0.42499999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="48303104"/>
-        <c:axId val="48317184"/>
+        <c:axId val="115760512"/>
+        <c:axId val="115770496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48303104"/>
+        <c:axId val="115760512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48317184"/>
+        <c:crossAx val="115770496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48317184"/>
+        <c:axId val="115770496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1073,7 +1073,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48303104"/>
+        <c:crossAx val="115760512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1082,7 +1082,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1133,39 +1133,39 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.96666666666666656</c:v>
+                  <c:v>0.82499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6333333333333333</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.86666666666666659</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="48332160"/>
-        <c:axId val="48350336"/>
+        <c:axId val="117112832"/>
+        <c:axId val="117114368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48332160"/>
+        <c:axId val="117112832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48350336"/>
+        <c:crossAx val="117114368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48350336"/>
+        <c:axId val="117114368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1173,7 +1173,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48332160"/>
+        <c:crossAx val="117112832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1182,7 +1182,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1371,10 +1371,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -1389,10 +1389,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -1401,13 +1401,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -1419,22 +1419,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>1</c:v>
@@ -1443,67 +1443,67 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>0</c:v>
@@ -1512,30 +1512,30 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="48451584"/>
-        <c:axId val="48453120"/>
+        <c:axId val="117141888"/>
+        <c:axId val="117143424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48451584"/>
+        <c:axId val="117141888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48453120"/>
+        <c:crossAx val="117143424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48453120"/>
+        <c:axId val="117143424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1545,7 +1545,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48451584"/>
+        <c:crossAx val="117141888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1554,7 +1554,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1602,24 +1602,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="48476544"/>
-        <c:axId val="48478080"/>
+        <c:axId val="118235904"/>
+        <c:axId val="118237440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48476544"/>
+        <c:axId val="118235904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48478080"/>
+        <c:crossAx val="118237440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48478080"/>
+        <c:axId val="118237440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1629,7 +1629,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48476544"/>
+        <c:crossAx val="118235904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1638,7 +1638,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1677,7 +1677,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>17.411764705882348</c:v>
+                  <c:v>19.583333333333332</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>84.095238095238102</c:v>
@@ -1686,24 +1686,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="49042560"/>
-        <c:axId val="49044096"/>
+        <c:axId val="118715904"/>
+        <c:axId val="118717440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="49042560"/>
+        <c:axId val="118715904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49044096"/>
+        <c:crossAx val="118717440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49044096"/>
+        <c:axId val="118717440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1711,7 +1711,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49042560"/>
+        <c:crossAx val="118715904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1720,7 +1720,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1768,42 +1768,42 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3.5555555555555554</c:v>
+                  <c:v>5.8214285714285712</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0277777777777777</c:v>
+                  <c:v>5.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.785714285714285</c:v>
+                  <c:v>32.80952380952381</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>131.08333333333334</c:v>
+                  <c:v>134.56944444444446</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>68.805555555555557</c:v>
+                  <c:v>70.083333333333329</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="49063424"/>
-        <c:axId val="49064960"/>
+        <c:axId val="118822784"/>
+        <c:axId val="118824320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="49063424"/>
+        <c:axId val="118822784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49064960"/>
+        <c:crossAx val="118824320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49064960"/>
+        <c:axId val="118824320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1811,7 +1811,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49063424"/>
+        <c:crossAx val="118822784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1820,7 +1820,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1871,39 +1871,39 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.25</c:v>
+                  <c:v>32.733333333333334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.75</c:v>
+                  <c:v>10.833333333333334</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>68.074074074074076</c:v>
+                  <c:v>68.648148148148152</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54.466666666666661</c:v>
+                  <c:v>55.216666666666661</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="48903680"/>
-        <c:axId val="48905216"/>
+        <c:axId val="118835072"/>
+        <c:axId val="118836608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48903680"/>
+        <c:axId val="118835072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48905216"/>
+        <c:crossAx val="118836608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48905216"/>
+        <c:axId val="118836608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1911,7 +1911,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48903680"/>
+        <c:crossAx val="118835072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1920,7 +1920,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2463,8 +2463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CX30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BA24" sqref="BA24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5001,6 +5001,311 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="1:102">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <v>0</v>
+      </c>
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8">
+        <v>0</v>
+      </c>
+      <c r="AM8">
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <v>0</v>
+      </c>
+      <c r="AO8">
+        <v>0</v>
+      </c>
+      <c r="AP8">
+        <v>0</v>
+      </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
+      <c r="AR8">
+        <v>0</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+      <c r="AT8">
+        <v>0</v>
+      </c>
+      <c r="AU8">
+        <v>0</v>
+      </c>
+      <c r="AV8">
+        <v>0</v>
+      </c>
+      <c r="AW8">
+        <v>0</v>
+      </c>
+      <c r="AX8">
+        <v>0</v>
+      </c>
+      <c r="AY8">
+        <v>0</v>
+      </c>
+      <c r="AZ8">
+        <v>0</v>
+      </c>
+      <c r="BA8">
+        <v>0</v>
+      </c>
+      <c r="BB8">
+        <v>0</v>
+      </c>
+      <c r="BC8">
+        <v>0</v>
+      </c>
+      <c r="BD8">
+        <v>0</v>
+      </c>
+      <c r="BE8">
+        <v>1</v>
+      </c>
+      <c r="BF8">
+        <v>0</v>
+      </c>
+      <c r="BG8">
+        <v>1</v>
+      </c>
+      <c r="BH8">
+        <v>0</v>
+      </c>
+      <c r="BI8">
+        <v>1</v>
+      </c>
+      <c r="BJ8">
+        <v>1</v>
+      </c>
+      <c r="BK8">
+        <v>0</v>
+      </c>
+      <c r="BL8">
+        <v>1</v>
+      </c>
+      <c r="BM8">
+        <v>0</v>
+      </c>
+      <c r="BN8">
+        <v>0</v>
+      </c>
+      <c r="BO8">
+        <v>1</v>
+      </c>
+      <c r="BP8">
+        <v>0</v>
+      </c>
+      <c r="BQ8">
+        <v>1</v>
+      </c>
+      <c r="BR8">
+        <v>0</v>
+      </c>
+      <c r="BS8">
+        <v>0</v>
+      </c>
+      <c r="BT8">
+        <v>0</v>
+      </c>
+      <c r="BU8">
+        <v>0</v>
+      </c>
+      <c r="BV8">
+        <v>1</v>
+      </c>
+      <c r="BW8">
+        <v>0</v>
+      </c>
+      <c r="BX8">
+        <v>1</v>
+      </c>
+      <c r="BY8">
+        <v>0</v>
+      </c>
+      <c r="BZ8">
+        <v>0</v>
+      </c>
+      <c r="CA8">
+        <v>0</v>
+      </c>
+      <c r="CB8">
+        <v>0</v>
+      </c>
+      <c r="CC8">
+        <v>0</v>
+      </c>
+      <c r="CD8">
+        <v>0</v>
+      </c>
+      <c r="CE8">
+        <v>0</v>
+      </c>
+      <c r="CF8">
+        <v>0</v>
+      </c>
+      <c r="CG8">
+        <v>0</v>
+      </c>
+      <c r="CH8">
+        <v>1</v>
+      </c>
+      <c r="CI8">
+        <v>1</v>
+      </c>
+      <c r="CJ8">
+        <v>0</v>
+      </c>
+      <c r="CK8">
+        <v>1</v>
+      </c>
+      <c r="CL8">
+        <v>0</v>
+      </c>
+      <c r="CM8">
+        <v>0</v>
+      </c>
+      <c r="CN8">
+        <v>1</v>
+      </c>
+      <c r="CO8">
+        <v>0</v>
+      </c>
+      <c r="CP8">
+        <v>0</v>
+      </c>
+      <c r="CQ8">
+        <v>0</v>
+      </c>
+      <c r="CR8">
+        <v>0</v>
+      </c>
+      <c r="CS8">
+        <v>0</v>
+      </c>
+      <c r="CT8">
+        <v>0</v>
+      </c>
+      <c r="CU8">
+        <v>1</v>
+      </c>
+      <c r="CV8">
+        <v>0</v>
+      </c>
+      <c r="CW8">
+        <v>0</v>
+      </c>
+      <c r="CX8">
+        <v>0</v>
+      </c>
+    </row>
     <row r="16" spans="1:102">
       <c r="C16" t="s">
         <v>31</v>
@@ -5017,11 +5322,11 @@
       </c>
       <c r="E17">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="F17">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G17">
         <f t="shared" si="13"/>
@@ -5041,11 +5346,11 @@
       </c>
       <c r="K17">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="L17">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="M17">
         <f t="shared" si="13"/>
@@ -5057,15 +5362,15 @@
       </c>
       <c r="O17">
         <f t="shared" si="13"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="P17">
         <f t="shared" si="13"/>
-        <v>0.66666666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="Q17">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="R17">
         <f t="shared" si="13"/>
@@ -5081,11 +5386,11 @@
       </c>
       <c r="U17">
         <f t="shared" si="13"/>
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="V17">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="W17">
         <f t="shared" si="13"/>
@@ -5093,15 +5398,15 @@
       </c>
       <c r="X17">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="Y17">
         <f t="shared" si="13"/>
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="Z17">
         <f t="shared" si="13"/>
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="AA17">
         <f t="shared" si="13"/>
@@ -5113,7 +5418,7 @@
       </c>
       <c r="AC17">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AD17">
         <f t="shared" si="13"/>
@@ -5121,11 +5426,11 @@
       </c>
       <c r="AE17">
         <f t="shared" si="13"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="AF17">
         <f t="shared" si="13"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="AG17">
         <f t="shared" si="13"/>
@@ -5133,7 +5438,7 @@
       </c>
       <c r="AH17">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AI17">
         <f t="shared" si="13"/>
@@ -5141,11 +5446,11 @@
       </c>
       <c r="AJ17">
         <f t="shared" si="13"/>
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="AK17">
         <f t="shared" si="13"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="AL17">
         <f t="shared" si="13"/>
@@ -5153,7 +5458,7 @@
       </c>
       <c r="AM17">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AN17">
         <f t="shared" si="13"/>
@@ -5161,11 +5466,11 @@
       </c>
       <c r="AO17">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AP17">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AQ17">
         <f t="shared" si="13"/>
@@ -5173,7 +5478,7 @@
       </c>
       <c r="AR17">
         <f t="shared" si="13"/>
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="AS17">
         <f t="shared" si="13"/>
@@ -5181,11 +5486,11 @@
       </c>
       <c r="AT17">
         <f t="shared" si="13"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="AU17">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AV17">
         <f t="shared" si="13"/>
@@ -5193,7 +5498,7 @@
       </c>
       <c r="AW17">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AX17">
         <f t="shared" si="13"/>
@@ -5205,7 +5510,7 @@
       </c>
       <c r="AZ17">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="19" spans="3:52">
@@ -5219,11 +5524,11 @@
     <row r="20" spans="3:52">
       <c r="C20">
         <f>AVERAGE(C17:AA17)</f>
-        <v>0.6</v>
+        <v>0.53</v>
       </c>
       <c r="D20">
         <f>AVERAGE(AB17:AZ17)</f>
-        <v>0.42666666666666664</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="22" spans="3:52">
@@ -5251,23 +5556,23 @@
     <row r="23" spans="3:52">
       <c r="C23">
         <f>AVERAGE(C17:G17,AB17:AF17)</f>
-        <v>0.46666666666666662</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="H23">
         <f>AVERAGE(H17:L17,AG17:AK17)</f>
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M23">
         <f>AVERAGE(M17:Q17,AL17:AP17)</f>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="R23">
         <f>AVERAGE(R17:V17,AQ17:AU17)</f>
-        <v>0.46666666666666662</v>
+        <v>0.375</v>
       </c>
       <c r="W23">
         <f>AVERAGE(W17:AA17,AV17:AZ17)</f>
-        <v>0.53333333333333333</v>
+        <v>0.42499999999999999</v>
       </c>
     </row>
     <row r="25" spans="3:52">
@@ -5299,7 +5604,7 @@
       </c>
       <c r="D26">
         <f t="shared" ref="D26:G26" si="15">AVERAGE(D17,I17,N17,S17,X17,AC17,AH17,AM17,AR17,AW17)</f>
-        <v>0.96666666666666656</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="E26">
         <f t="shared" si="15"/>
@@ -5307,11 +5612,11 @@
       </c>
       <c r="F26">
         <f t="shared" si="15"/>
-        <v>0.6333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="G26">
         <f t="shared" si="15"/>
-        <v>0.86666666666666659</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="29" spans="3:52">
@@ -5344,8 +5649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CX56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AZ46" sqref="AZ46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8014,6 +8319,311 @@
         <v>931</v>
       </c>
     </row>
+    <row r="8" spans="1:102">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>-1</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>19</v>
+      </c>
+      <c r="F8">
+        <v>-1</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>-1</v>
+      </c>
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <v>-1</v>
+      </c>
+      <c r="K8">
+        <v>-1</v>
+      </c>
+      <c r="L8">
+        <v>-1</v>
+      </c>
+      <c r="M8">
+        <v>-1</v>
+      </c>
+      <c r="N8">
+        <v>10</v>
+      </c>
+      <c r="O8">
+        <v>-1</v>
+      </c>
+      <c r="P8">
+        <v>18</v>
+      </c>
+      <c r="Q8">
+        <v>-1</v>
+      </c>
+      <c r="R8">
+        <v>-1</v>
+      </c>
+      <c r="S8">
+        <v>103</v>
+      </c>
+      <c r="T8">
+        <v>-1</v>
+      </c>
+      <c r="U8">
+        <v>-1</v>
+      </c>
+      <c r="V8">
+        <v>-1</v>
+      </c>
+      <c r="W8">
+        <v>-1</v>
+      </c>
+      <c r="X8">
+        <v>-1</v>
+      </c>
+      <c r="Y8">
+        <v>-1</v>
+      </c>
+      <c r="Z8">
+        <v>-1</v>
+      </c>
+      <c r="AA8">
+        <v>35</v>
+      </c>
+      <c r="AB8">
+        <v>-1</v>
+      </c>
+      <c r="AC8">
+        <v>-1</v>
+      </c>
+      <c r="AD8">
+        <v>-1</v>
+      </c>
+      <c r="AE8">
+        <v>-1</v>
+      </c>
+      <c r="AF8">
+        <v>-1</v>
+      </c>
+      <c r="AG8">
+        <v>-1</v>
+      </c>
+      <c r="AH8">
+        <v>-1</v>
+      </c>
+      <c r="AI8">
+        <v>-1</v>
+      </c>
+      <c r="AJ8">
+        <v>-1</v>
+      </c>
+      <c r="AK8">
+        <v>-1</v>
+      </c>
+      <c r="AL8">
+        <v>-1</v>
+      </c>
+      <c r="AM8">
+        <v>-1</v>
+      </c>
+      <c r="AN8">
+        <v>-1</v>
+      </c>
+      <c r="AO8">
+        <v>-1</v>
+      </c>
+      <c r="AP8">
+        <v>-1</v>
+      </c>
+      <c r="AQ8">
+        <v>-1</v>
+      </c>
+      <c r="AR8">
+        <v>-1</v>
+      </c>
+      <c r="AS8">
+        <v>-1</v>
+      </c>
+      <c r="AT8">
+        <v>-1</v>
+      </c>
+      <c r="AU8">
+        <v>-1</v>
+      </c>
+      <c r="AV8">
+        <v>-1</v>
+      </c>
+      <c r="AW8">
+        <v>-1</v>
+      </c>
+      <c r="AX8">
+        <v>-1</v>
+      </c>
+      <c r="AY8">
+        <v>-1</v>
+      </c>
+      <c r="AZ8">
+        <v>-1</v>
+      </c>
+      <c r="BA8">
+        <v>-1</v>
+      </c>
+      <c r="BB8">
+        <v>-1</v>
+      </c>
+      <c r="BC8">
+        <v>-1</v>
+      </c>
+      <c r="BD8">
+        <v>-1</v>
+      </c>
+      <c r="BE8">
+        <v>10</v>
+      </c>
+      <c r="BF8">
+        <v>-1</v>
+      </c>
+      <c r="BG8">
+        <v>8</v>
+      </c>
+      <c r="BH8">
+        <v>-1</v>
+      </c>
+      <c r="BI8">
+        <v>8</v>
+      </c>
+      <c r="BJ8">
+        <v>4</v>
+      </c>
+      <c r="BK8">
+        <v>-1</v>
+      </c>
+      <c r="BL8">
+        <v>8</v>
+      </c>
+      <c r="BM8">
+        <v>-1</v>
+      </c>
+      <c r="BN8">
+        <v>-1</v>
+      </c>
+      <c r="BO8">
+        <v>7</v>
+      </c>
+      <c r="BP8">
+        <v>-1</v>
+      </c>
+      <c r="BQ8">
+        <v>347</v>
+      </c>
+      <c r="BR8">
+        <v>-1</v>
+      </c>
+      <c r="BS8">
+        <v>-1</v>
+      </c>
+      <c r="BT8">
+        <v>-1</v>
+      </c>
+      <c r="BU8">
+        <v>-1</v>
+      </c>
+      <c r="BV8">
+        <v>30</v>
+      </c>
+      <c r="BW8">
+        <v>-1</v>
+      </c>
+      <c r="BX8">
+        <v>231</v>
+      </c>
+      <c r="BY8">
+        <v>-1</v>
+      </c>
+      <c r="BZ8">
+        <v>-1</v>
+      </c>
+      <c r="CA8">
+        <v>-1</v>
+      </c>
+      <c r="CB8">
+        <v>-1</v>
+      </c>
+      <c r="CC8">
+        <v>-1</v>
+      </c>
+      <c r="CD8">
+        <v>-1</v>
+      </c>
+      <c r="CE8">
+        <v>-1</v>
+      </c>
+      <c r="CF8">
+        <v>-1</v>
+      </c>
+      <c r="CG8">
+        <v>-1</v>
+      </c>
+      <c r="CH8">
+        <v>444</v>
+      </c>
+      <c r="CI8">
+        <v>551</v>
+      </c>
+      <c r="CJ8">
+        <v>-1</v>
+      </c>
+      <c r="CK8">
+        <v>2</v>
+      </c>
+      <c r="CL8">
+        <v>-1</v>
+      </c>
+      <c r="CM8">
+        <v>-1</v>
+      </c>
+      <c r="CN8">
+        <v>7</v>
+      </c>
+      <c r="CO8">
+        <v>-1</v>
+      </c>
+      <c r="CP8">
+        <v>-1</v>
+      </c>
+      <c r="CQ8">
+        <v>-1</v>
+      </c>
+      <c r="CR8">
+        <v>-1</v>
+      </c>
+      <c r="CS8">
+        <v>-1</v>
+      </c>
+      <c r="CT8">
+        <v>-1</v>
+      </c>
+      <c r="CU8">
+        <v>186</v>
+      </c>
+      <c r="CV8">
+        <v>-1</v>
+      </c>
+      <c r="CW8">
+        <v>-1</v>
+      </c>
+      <c r="CX8">
+        <v>-1</v>
+      </c>
+    </row>
     <row r="22" spans="3:102">
       <c r="C22" t="str">
         <f>IF(C6&gt;=0,C6,"")</f>
@@ -8819,405 +9429,405 @@
       </c>
     </row>
     <row r="24" spans="3:102">
-      <c r="C24">
+      <c r="C24" t="str">
         <f t="shared" ref="C24:BN24" si="4">IF(C8&gt;=0,C8,"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D24">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E24">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F24">
+        <v>19</v>
+      </c>
+      <c r="F24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="G24">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H24">
+        <v>3</v>
+      </c>
+      <c r="H24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="I24">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J24">
+        <v>7</v>
+      </c>
+      <c r="J24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K24">
+        <v/>
+      </c>
+      <c r="K24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L24">
+        <v/>
+      </c>
+      <c r="L24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M24">
+        <v/>
+      </c>
+      <c r="M24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="N24">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O24">
+        <v>10</v>
+      </c>
+      <c r="O24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="P24">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q24">
+        <v>18</v>
+      </c>
+      <c r="Q24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="R24">
+        <v/>
+      </c>
+      <c r="R24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="S24">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T24">
+        <v>103</v>
+      </c>
+      <c r="T24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="U24">
+        <v/>
+      </c>
+      <c r="U24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V24">
+        <v/>
+      </c>
+      <c r="V24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="W24">
+        <v/>
+      </c>
+      <c r="W24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X24">
+        <v/>
+      </c>
+      <c r="X24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y24">
+        <v/>
+      </c>
+      <c r="Y24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Z24">
+        <v/>
+      </c>
+      <c r="Z24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AA24">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB24">
+        <v>35</v>
+      </c>
+      <c r="AB24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AC24">
+        <v/>
+      </c>
+      <c r="AC24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AD24">
+        <v/>
+      </c>
+      <c r="AD24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AE24">
+        <v/>
+      </c>
+      <c r="AE24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AF24">
+        <v/>
+      </c>
+      <c r="AF24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AG24">
+        <v/>
+      </c>
+      <c r="AG24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AH24">
+        <v/>
+      </c>
+      <c r="AH24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AI24">
+        <v/>
+      </c>
+      <c r="AI24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AJ24">
+        <v/>
+      </c>
+      <c r="AJ24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AK24">
+        <v/>
+      </c>
+      <c r="AK24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AL24">
+        <v/>
+      </c>
+      <c r="AL24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AM24">
+        <v/>
+      </c>
+      <c r="AM24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AN24">
+        <v/>
+      </c>
+      <c r="AN24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AO24">
+        <v/>
+      </c>
+      <c r="AO24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AP24">
+        <v/>
+      </c>
+      <c r="AP24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AQ24">
+        <v/>
+      </c>
+      <c r="AQ24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AR24">
+        <v/>
+      </c>
+      <c r="AR24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AS24">
+        <v/>
+      </c>
+      <c r="AS24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AT24">
+        <v/>
+      </c>
+      <c r="AT24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AU24">
+        <v/>
+      </c>
+      <c r="AU24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AV24">
+        <v/>
+      </c>
+      <c r="AV24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AW24">
+        <v/>
+      </c>
+      <c r="AW24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AX24">
+        <v/>
+      </c>
+      <c r="AX24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AY24">
+        <v/>
+      </c>
+      <c r="AY24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AZ24">
+        <v/>
+      </c>
+      <c r="AZ24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="BA24">
+        <v/>
+      </c>
+      <c r="BA24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="BB24">
+        <v/>
+      </c>
+      <c r="BB24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="BC24">
+        <v/>
+      </c>
+      <c r="BC24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="BD24">
+        <v/>
+      </c>
+      <c r="BD24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BE24">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="BF24">
+        <v>10</v>
+      </c>
+      <c r="BF24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BG24">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="BH24">
+        <v>8</v>
+      </c>
+      <c r="BH24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BI24">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="BJ24">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="BK24">
+        <v>4</v>
+      </c>
+      <c r="BK24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BL24">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="BM24">
+        <v>8</v>
+      </c>
+      <c r="BM24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="BN24">
+        <v/>
+      </c>
+      <c r="BN24" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BO24">
         <f t="shared" ref="BO24:CX24" si="5">IF(BO8&gt;=0,BO8,"")</f>
-        <v>0</v>
-      </c>
-      <c r="BP24">
+        <v>7</v>
+      </c>
+      <c r="BP24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BQ24">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="BR24">
+        <v>347</v>
+      </c>
+      <c r="BR24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="BS24">
+        <v/>
+      </c>
+      <c r="BS24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="BT24">
+        <v/>
+      </c>
+      <c r="BT24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="BU24">
+        <v/>
+      </c>
+      <c r="BU24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BV24">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="BW24">
+        <v>30</v>
+      </c>
+      <c r="BW24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BX24">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="BY24">
+        <v>231</v>
+      </c>
+      <c r="BY24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="BZ24">
+        <v/>
+      </c>
+      <c r="BZ24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="CA24">
+        <v/>
+      </c>
+      <c r="CA24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="CB24">
+        <v/>
+      </c>
+      <c r="CB24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="CC24">
+        <v/>
+      </c>
+      <c r="CC24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="CD24">
+        <v/>
+      </c>
+      <c r="CD24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="CE24">
+        <v/>
+      </c>
+      <c r="CE24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="CF24">
+        <v/>
+      </c>
+      <c r="CF24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="CG24">
+        <v/>
+      </c>
+      <c r="CG24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CH24">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>444</v>
       </c>
       <c r="CI24">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="CJ24">
+        <v>551</v>
+      </c>
+      <c r="CJ24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CK24">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="CL24">
+        <v>2</v>
+      </c>
+      <c r="CL24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="CM24">
+        <v/>
+      </c>
+      <c r="CM24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CN24">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="CO24">
+        <v>7</v>
+      </c>
+      <c r="CO24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="CP24">
+        <v/>
+      </c>
+      <c r="CP24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="CQ24">
+        <v/>
+      </c>
+      <c r="CQ24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="CR24">
+        <v/>
+      </c>
+      <c r="CR24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="CS24">
+        <v/>
+      </c>
+      <c r="CS24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="CT24">
+        <v/>
+      </c>
+      <c r="CT24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CU24">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="CV24">
+        <v>186</v>
+      </c>
+      <c r="CV24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="CW24">
+        <v/>
+      </c>
+      <c r="CW24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="CX24">
+        <v/>
+      </c>
+      <c r="CX24" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="25" spans="3:102">
@@ -12845,16 +13455,16 @@
     </row>
     <row r="43" spans="3:102">
       <c r="C43" t="e">
-        <f>AVERAGE(C22:C23,BA22)</f>
+        <f>AVERAGE(C22:C24,BA22)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D43">
-        <f t="shared" ref="D43:AZ43" si="24">AVERAGE(D22:D23,BB22)</f>
-        <v>3.6666666666666665</v>
-      </c>
-      <c r="E43" t="e">
+        <f t="shared" ref="D43:AZ43" si="24">AVERAGE(D22:D24,BB22)</f>
+        <v>4.25</v>
+      </c>
+      <c r="E43">
         <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
+        <v>19</v>
       </c>
       <c r="F43">
         <f t="shared" si="24"/>
@@ -12862,7 +13472,7 @@
       </c>
       <c r="G43">
         <f t="shared" si="24"/>
-        <v>3.6666666666666665</v>
+        <v>3.5</v>
       </c>
       <c r="H43" t="e">
         <f t="shared" si="24"/>
@@ -12870,7 +13480,7 @@
       </c>
       <c r="I43">
         <f t="shared" si="24"/>
-        <v>1.6666666666666667</v>
+        <v>3</v>
       </c>
       <c r="J43" t="e">
         <f t="shared" si="24"/>
@@ -12890,7 +13500,7 @@
       </c>
       <c r="N43">
         <f t="shared" si="24"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O43">
         <f t="shared" si="24"/>
@@ -12898,7 +13508,7 @@
       </c>
       <c r="P43">
         <f t="shared" si="24"/>
-        <v>2.5</v>
+        <v>7.666666666666667</v>
       </c>
       <c r="Q43">
         <f t="shared" si="24"/>
@@ -12910,7 +13520,7 @@
       </c>
       <c r="S43">
         <f t="shared" si="24"/>
-        <v>19.333333333333332</v>
+        <v>40.25</v>
       </c>
       <c r="T43" t="e">
         <f t="shared" si="24"/>
@@ -12942,7 +13552,7 @@
       </c>
       <c r="AA43">
         <f t="shared" si="24"/>
-        <v>4.333333333333333</v>
+        <v>12</v>
       </c>
       <c r="AB43" t="e">
         <f t="shared" si="24"/>
@@ -13052,11 +13662,11 @@
       </c>
       <c r="D44">
         <f t="shared" ref="D44:AZ44" si="25">IF(ISNUMBER(D43),D43,"")</f>
-        <v>3.6666666666666665</v>
-      </c>
-      <c r="E44" t="str">
+        <v>4.25</v>
+      </c>
+      <c r="E44">
         <f t="shared" si="25"/>
-        <v/>
+        <v>19</v>
       </c>
       <c r="F44">
         <f t="shared" si="25"/>
@@ -13064,7 +13674,7 @@
       </c>
       <c r="G44">
         <f t="shared" si="25"/>
-        <v>3.6666666666666665</v>
+        <v>3.5</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="25"/>
@@ -13072,7 +13682,7 @@
       </c>
       <c r="I44">
         <f t="shared" si="25"/>
-        <v>1.6666666666666667</v>
+        <v>3</v>
       </c>
       <c r="J44" t="str">
         <f t="shared" si="25"/>
@@ -13092,7 +13702,7 @@
       </c>
       <c r="N44">
         <f t="shared" si="25"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O44">
         <f t="shared" si="25"/>
@@ -13100,7 +13710,7 @@
       </c>
       <c r="P44">
         <f t="shared" si="25"/>
-        <v>2.5</v>
+        <v>7.666666666666667</v>
       </c>
       <c r="Q44">
         <f t="shared" si="25"/>
@@ -13112,7 +13722,7 @@
       </c>
       <c r="S44">
         <f t="shared" si="25"/>
-        <v>19.333333333333332</v>
+        <v>40.25</v>
       </c>
       <c r="T44" t="str">
         <f t="shared" si="25"/>
@@ -13144,7 +13754,7 @@
       </c>
       <c r="AA44">
         <f t="shared" si="25"/>
-        <v>4.333333333333333</v>
+        <v>12</v>
       </c>
       <c r="AB44" t="str">
         <f t="shared" si="25"/>
@@ -13258,7 +13868,7 @@
     <row r="49" spans="3:23">
       <c r="C49">
         <f>AVERAGE(C44:AA44)</f>
-        <v>17.411764705882348</v>
+        <v>19.583333333333332</v>
       </c>
       <c r="D49">
         <f>AVERAGE(AB44:AZ44)</f>
@@ -13290,23 +13900,23 @@
     <row r="52" spans="3:23">
       <c r="C52">
         <f>AVERAGE(C44:G44,AB44:AF44)</f>
-        <v>3.5555555555555554</v>
+        <v>5.8214285714285712</v>
       </c>
       <c r="H52">
         <f>AVERAGE(H44:L44,AG44:AK44)</f>
-        <v>5.0277777777777777</v>
+        <v>5.25</v>
       </c>
       <c r="M52">
         <f>AVERAGE(M44:Q44,AL44:AP44)</f>
-        <v>31.785714285714285</v>
+        <v>32.80952380952381</v>
       </c>
       <c r="R52">
         <f>AVERAGE(R44:V44,AQ44:AU44)</f>
-        <v>131.08333333333334</v>
+        <v>134.56944444444446</v>
       </c>
       <c r="W52">
         <f>AVERAGE(W44:AA44,AV44:AZ44)</f>
-        <v>68.805555555555557</v>
+        <v>70.083333333333329</v>
       </c>
     </row>
     <row r="55" spans="3:23">
@@ -13338,19 +13948,19 @@
       </c>
       <c r="D56">
         <f>AVERAGE(D44,I44,N44,S44,X44,AC44,AH44,AM44,AR44,AW44)</f>
-        <v>30.25</v>
+        <v>32.733333333333334</v>
       </c>
       <c r="E56">
         <f>AVERAGE(E44,J44,O44,T44,Y44,AD44,AI44,AN44,AS44,AX44)</f>
-        <v>6.75</v>
+        <v>10.833333333333334</v>
       </c>
       <c r="F56">
         <f>AVERAGE(F44,K44,P44,U44,Z44,AE44,AJ44,AO44,AT44,AY44)</f>
-        <v>68.074074074074076</v>
+        <v>68.648148148148152</v>
       </c>
       <c r="G56">
         <f>AVERAGE(G44,L44,Q44,V44,AA44,AF44,AK44,AP44,AU44,AZ44)</f>
-        <v>54.466666666666661</v>
+        <v>55.216666666666661</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pilot 1 - User 4.
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -850,8 +850,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -935,33 +936,33 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.53</c:v>
+                  <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32</c:v>
+                  <c:v>0.32800000000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="115739648"/>
-        <c:axId val="115741440"/>
+        <c:axId val="50313856"/>
+        <c:axId val="50323840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115739648"/>
+        <c:axId val="50313856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115741440"/>
+        <c:crossAx val="50323840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115741440"/>
+        <c:axId val="50323840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -971,7 +972,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115739648"/>
+        <c:crossAx val="50313856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -980,7 +981,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1028,42 +1029,42 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.42499999999999999</c:v>
+                  <c:v>0.44000000000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5</c:v>
+                  <c:v>0.49999999999999989</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.375</c:v>
+                  <c:v>0.34</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.42499999999999999</c:v>
+                  <c:v>0.44000000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="115760512"/>
-        <c:axId val="115770496"/>
+        <c:axId val="50203648"/>
+        <c:axId val="50217728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115760512"/>
+        <c:axId val="50203648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115770496"/>
+        <c:crossAx val="50217728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115770496"/>
+        <c:axId val="50217728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1073,7 +1074,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115760512"/>
+        <c:crossAx val="50203648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1082,7 +1083,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1133,39 +1134,39 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.82499999999999996</c:v>
+                  <c:v>0.79999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5</c:v>
+                  <c:v>0.50000000000000011</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7</c:v>
+                  <c:v>0.72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="117112832"/>
-        <c:axId val="117114368"/>
+        <c:axId val="50228608"/>
+        <c:axId val="50250880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="117112832"/>
+        <c:axId val="50228608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117114368"/>
+        <c:crossAx val="50250880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117114368"/>
+        <c:axId val="50250880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1173,7 +1174,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117112832"/>
+        <c:crossAx val="50228608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1182,7 +1183,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1371,10 +1372,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.75</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -1389,10 +1390,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.75</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.75</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -1401,13 +1402,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.25</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.75</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.75</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -1419,22 +1420,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.75</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.75</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.5</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>1</c:v>
@@ -1443,99 +1444,99 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.75</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.25</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.25</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.75</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.25</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.75</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.75</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.75</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.25</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.75</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.75</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.75</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="117141888"/>
-        <c:axId val="117143424"/>
+        <c:axId val="50352128"/>
+        <c:axId val="50353664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="117141888"/>
+        <c:axId val="50352128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117143424"/>
+        <c:crossAx val="50353664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117143424"/>
+        <c:axId val="50353664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1545,7 +1546,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117141888"/>
+        <c:crossAx val="50352128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1554,7 +1555,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1602,24 +1603,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="118235904"/>
-        <c:axId val="118237440"/>
+        <c:axId val="50377088"/>
+        <c:axId val="50378624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="118235904"/>
+        <c:axId val="50377088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118237440"/>
+        <c:crossAx val="50378624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118237440"/>
+        <c:axId val="50378624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1629,7 +1630,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118235904"/>
+        <c:crossAx val="50377088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1638,7 +1639,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1677,33 +1678,33 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>19.583333333333332</c:v>
+                  <c:v>16.725000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>84.095238095238102</c:v>
+                  <c:v>71.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="118715904"/>
-        <c:axId val="118717440"/>
+        <c:axId val="50803840"/>
+        <c:axId val="50805376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="118715904"/>
+        <c:axId val="50803840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118717440"/>
+        <c:crossAx val="50805376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118717440"/>
+        <c:axId val="50805376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1711,7 +1712,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118715904"/>
+        <c:crossAx val="50803840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1720,7 +1721,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1768,42 +1769,42 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5.8214285714285712</c:v>
+                  <c:v>5.6520833333333336</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.25</c:v>
+                  <c:v>4.9916666666666663</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32.80952380952381</c:v>
+                  <c:v>25.966666666666665</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>134.56944444444446</c:v>
+                  <c:v>132.99722222222223</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70.083333333333329</c:v>
+                  <c:v>56.304761904761904</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="118822784"/>
-        <c:axId val="118824320"/>
+        <c:axId val="50832896"/>
+        <c:axId val="50834432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="118822784"/>
+        <c:axId val="50832896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118824320"/>
+        <c:crossAx val="50834432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118824320"/>
+        <c:axId val="50834432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1811,7 +1812,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118822784"/>
+        <c:crossAx val="50832896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1820,7 +1821,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1871,39 +1872,39 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.733333333333334</c:v>
+                  <c:v>31.175000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.833333333333334</c:v>
+                  <c:v>8.375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>68.648148148148152</c:v>
+                  <c:v>63.341666666666676</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55.216666666666661</c:v>
+                  <c:v>47.038333333333334</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="118835072"/>
-        <c:axId val="118836608"/>
+        <c:axId val="51058176"/>
+        <c:axId val="51059712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="118835072"/>
+        <c:axId val="51058176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118836608"/>
+        <c:crossAx val="51059712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118836608"/>
+        <c:axId val="51059712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1911,7 +1912,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118835072"/>
+        <c:crossAx val="51058176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1920,7 +1921,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2461,10 +2462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CX30"/>
+  <dimension ref="A1:DA30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T34" sqref="T34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2489,7 +2490,7 @@
     <col min="54" max="102" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:102">
+    <row r="1" spans="1:105">
       <c r="C1" t="s">
         <v>26</v>
       </c>
@@ -2889,7 +2890,7 @@
         <v>Repetition 2</v>
       </c>
     </row>
-    <row r="2" spans="1:102">
+    <row r="2" spans="1:105">
       <c r="C2" t="s">
         <v>28</v>
       </c>
@@ -3289,7 +3290,7 @@
         <v>Peripheral</v>
       </c>
     </row>
-    <row r="3" spans="1:102">
+    <row r="3" spans="1:105">
       <c r="C3" t="s">
         <v>33</v>
       </c>
@@ -3686,7 +3687,7 @@
         <v>Duration 500</v>
       </c>
     </row>
-    <row r="4" spans="1:102">
+    <row r="4" spans="1:105">
       <c r="C4" t="s">
         <v>30</v>
       </c>
@@ -4083,7 +4084,7 @@
         <v>Amplitude 75</v>
       </c>
     </row>
-    <row r="5" spans="1:102">
+    <row r="5" spans="1:105">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -4391,7 +4392,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:102">
+    <row r="6" spans="1:105">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4695,8 +4696,12 @@
       <c r="CX6">
         <v>1</v>
       </c>
+      <c r="DA6" s="1">
+        <f>SUM(C6:CX6)</f>
+        <v>52</v>
+      </c>
     </row>
-    <row r="7" spans="1:102">
+    <row r="7" spans="1:105">
       <c r="A7">
         <v>2</v>
       </c>
@@ -5000,8 +5005,12 @@
       <c r="CX7">
         <v>1</v>
       </c>
+      <c r="DA7" s="1">
+        <f t="shared" ref="DA7:DA9" si="13">SUM(C7:CX7)</f>
+        <v>52</v>
+      </c>
     </row>
-    <row r="8" spans="1:102">
+    <row r="8" spans="1:105">
       <c r="A8">
         <v>3</v>
       </c>
@@ -5305,8 +5314,321 @@
       <c r="CX8">
         <v>0</v>
       </c>
+      <c r="DA8" s="1">
+        <f t="shared" si="13"/>
+        <v>22</v>
+      </c>
     </row>
-    <row r="16" spans="1:102">
+    <row r="9" spans="1:105">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>1</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>1</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>1</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>1</v>
+      </c>
+      <c r="AG9">
+        <v>0</v>
+      </c>
+      <c r="AH9">
+        <v>1</v>
+      </c>
+      <c r="AI9">
+        <v>0</v>
+      </c>
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <v>0</v>
+      </c>
+      <c r="AM9">
+        <v>1</v>
+      </c>
+      <c r="AN9">
+        <v>0</v>
+      </c>
+      <c r="AO9">
+        <v>1</v>
+      </c>
+      <c r="AP9">
+        <v>1</v>
+      </c>
+      <c r="AQ9">
+        <v>0</v>
+      </c>
+      <c r="AR9">
+        <v>0</v>
+      </c>
+      <c r="AS9">
+        <v>0</v>
+      </c>
+      <c r="AT9">
+        <v>0</v>
+      </c>
+      <c r="AU9">
+        <v>1</v>
+      </c>
+      <c r="AV9">
+        <v>0</v>
+      </c>
+      <c r="AW9">
+        <v>0</v>
+      </c>
+      <c r="AX9">
+        <v>0</v>
+      </c>
+      <c r="AY9">
+        <v>1</v>
+      </c>
+      <c r="AZ9">
+        <v>1</v>
+      </c>
+      <c r="BA9">
+        <v>0</v>
+      </c>
+      <c r="BB9">
+        <v>1</v>
+      </c>
+      <c r="BC9">
+        <v>0</v>
+      </c>
+      <c r="BD9">
+        <v>1</v>
+      </c>
+      <c r="BE9">
+        <v>1</v>
+      </c>
+      <c r="BF9">
+        <v>0</v>
+      </c>
+      <c r="BG9">
+        <v>1</v>
+      </c>
+      <c r="BH9">
+        <v>0</v>
+      </c>
+      <c r="BI9">
+        <v>0</v>
+      </c>
+      <c r="BJ9">
+        <v>1</v>
+      </c>
+      <c r="BK9">
+        <v>0</v>
+      </c>
+      <c r="BL9">
+        <v>1</v>
+      </c>
+      <c r="BM9">
+        <v>0</v>
+      </c>
+      <c r="BN9">
+        <v>1</v>
+      </c>
+      <c r="BO9">
+        <v>1</v>
+      </c>
+      <c r="BP9">
+        <v>0</v>
+      </c>
+      <c r="BQ9">
+        <v>1</v>
+      </c>
+      <c r="BR9">
+        <v>0</v>
+      </c>
+      <c r="BS9">
+        <v>1</v>
+      </c>
+      <c r="BT9">
+        <v>1</v>
+      </c>
+      <c r="BU9">
+        <v>0</v>
+      </c>
+      <c r="BV9">
+        <v>1</v>
+      </c>
+      <c r="BW9">
+        <v>1</v>
+      </c>
+      <c r="BX9">
+        <v>0</v>
+      </c>
+      <c r="BY9">
+        <v>1</v>
+      </c>
+      <c r="BZ9">
+        <v>0</v>
+      </c>
+      <c r="CA9">
+        <v>1</v>
+      </c>
+      <c r="CB9">
+        <v>0</v>
+      </c>
+      <c r="CC9">
+        <v>0</v>
+      </c>
+      <c r="CD9">
+        <v>0</v>
+      </c>
+      <c r="CE9">
+        <v>0</v>
+      </c>
+      <c r="CF9">
+        <v>1</v>
+      </c>
+      <c r="CG9">
+        <v>0</v>
+      </c>
+      <c r="CH9">
+        <v>1</v>
+      </c>
+      <c r="CI9">
+        <v>0</v>
+      </c>
+      <c r="CJ9">
+        <v>0</v>
+      </c>
+      <c r="CK9">
+        <v>1</v>
+      </c>
+      <c r="CL9">
+        <v>1</v>
+      </c>
+      <c r="CM9">
+        <v>0</v>
+      </c>
+      <c r="CN9">
+        <v>1</v>
+      </c>
+      <c r="CO9">
+        <v>0</v>
+      </c>
+      <c r="CP9">
+        <v>0</v>
+      </c>
+      <c r="CQ9">
+        <v>0</v>
+      </c>
+      <c r="CR9">
+        <v>0</v>
+      </c>
+      <c r="CS9">
+        <v>1</v>
+      </c>
+      <c r="CT9">
+        <v>0</v>
+      </c>
+      <c r="CU9">
+        <v>1</v>
+      </c>
+      <c r="CV9">
+        <v>0</v>
+      </c>
+      <c r="CW9">
+        <v>1</v>
+      </c>
+      <c r="CX9">
+        <v>0</v>
+      </c>
+      <c r="DA9" s="1">
+        <f t="shared" si="13"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:105">
       <c r="C16" t="s">
         <v>31</v>
       </c>
@@ -5317,200 +5639,200 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <f t="shared" ref="D17:AZ17" si="13">AVERAGE(D6:D14,BB6)</f>
+        <f t="shared" ref="D17:AZ17" si="14">AVERAGE(D6:D14,BB6)</f>
         <v>1</v>
       </c>
       <c r="E17">
-        <f t="shared" si="13"/>
-        <v>0.25</v>
+        <f t="shared" si="14"/>
+        <v>0.2</v>
       </c>
       <c r="F17">
-        <f t="shared" si="13"/>
-        <v>0.75</v>
+        <f t="shared" si="14"/>
+        <v>0.8</v>
       </c>
       <c r="G17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="H17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="J17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K17">
-        <f t="shared" si="13"/>
-        <v>0.75</v>
+        <f t="shared" si="14"/>
+        <v>0.8</v>
       </c>
       <c r="L17">
-        <f t="shared" si="13"/>
-        <v>0.75</v>
+        <f t="shared" si="14"/>
+        <v>0.8</v>
       </c>
       <c r="M17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="O17">
-        <f t="shared" si="13"/>
-        <v>0.25</v>
+        <f t="shared" si="14"/>
+        <v>0.2</v>
       </c>
       <c r="P17">
-        <f t="shared" si="13"/>
-        <v>0.75</v>
+        <f t="shared" si="14"/>
+        <v>0.6</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="13"/>
-        <v>0.75</v>
+        <f t="shared" si="14"/>
+        <v>0.8</v>
       </c>
       <c r="R17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="U17">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
+        <f t="shared" si="14"/>
+        <v>0.4</v>
       </c>
       <c r="V17">
-        <f t="shared" si="13"/>
-        <v>0.75</v>
+        <f t="shared" si="14"/>
+        <v>0.6</v>
       </c>
       <c r="W17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X17">
-        <f t="shared" si="13"/>
-        <v>0.75</v>
+        <f t="shared" si="14"/>
+        <v>0.8</v>
       </c>
       <c r="Y17">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
+        <f t="shared" si="14"/>
+        <v>0.4</v>
       </c>
       <c r="Z17">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
+        <f t="shared" si="14"/>
+        <v>0.6</v>
       </c>
       <c r="AA17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AB17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AC17">
-        <f t="shared" si="13"/>
-        <v>0.75</v>
+        <f t="shared" si="14"/>
+        <v>0.6</v>
       </c>
       <c r="AD17">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>0.2</v>
       </c>
       <c r="AE17">
-        <f t="shared" si="13"/>
-        <v>0.25</v>
+        <f t="shared" si="14"/>
+        <v>0.2</v>
       </c>
       <c r="AF17">
-        <f t="shared" si="13"/>
-        <v>0.25</v>
+        <f t="shared" si="14"/>
+        <v>0.4</v>
       </c>
       <c r="AG17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH17">
-        <f t="shared" si="13"/>
-        <v>0.75</v>
+        <f t="shared" si="14"/>
+        <v>0.8</v>
       </c>
       <c r="AI17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ17">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
+        <f t="shared" si="14"/>
+        <v>0.4</v>
       </c>
       <c r="AK17">
-        <f t="shared" si="13"/>
-        <v>0.25</v>
+        <f t="shared" si="14"/>
+        <v>0.2</v>
       </c>
       <c r="AL17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AM17">
-        <f t="shared" si="13"/>
-        <v>0.75</v>
+        <f t="shared" si="14"/>
+        <v>0.8</v>
       </c>
       <c r="AN17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AO17">
-        <f t="shared" si="13"/>
-        <v>0.75</v>
+        <f t="shared" si="14"/>
+        <v>0.8</v>
       </c>
       <c r="AP17">
-        <f t="shared" si="13"/>
-        <v>0.75</v>
+        <f t="shared" si="14"/>
+        <v>0.8</v>
       </c>
       <c r="AQ17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AR17">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
+        <f t="shared" si="14"/>
+        <v>0.4</v>
       </c>
       <c r="AS17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AT17">
-        <f t="shared" si="13"/>
-        <v>0.25</v>
+        <f t="shared" si="14"/>
+        <v>0.2</v>
       </c>
       <c r="AU17">
-        <f t="shared" si="13"/>
-        <v>0.75</v>
+        <f t="shared" si="14"/>
+        <v>0.8</v>
       </c>
       <c r="AV17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AW17">
-        <f t="shared" si="13"/>
-        <v>0.75</v>
+        <f t="shared" si="14"/>
+        <v>0.6</v>
       </c>
       <c r="AX17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AY17">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>0.2</v>
       </c>
       <c r="AZ17">
-        <f t="shared" si="13"/>
-        <v>0.75</v>
+        <f t="shared" si="14"/>
+        <v>0.8</v>
       </c>
     </row>
     <row r="19" spans="3:52">
@@ -5524,11 +5846,11 @@
     <row r="20" spans="3:52">
       <c r="C20">
         <f>AVERAGE(C17:AA17)</f>
-        <v>0.53</v>
+        <v>0.52</v>
       </c>
       <c r="D20">
         <f>AVERAGE(AB17:AZ17)</f>
-        <v>0.32</v>
+        <v>0.32800000000000007</v>
       </c>
     </row>
     <row r="22" spans="3:52">
@@ -5556,7 +5878,7 @@
     <row r="23" spans="3:52">
       <c r="C23">
         <f>AVERAGE(C17:G17,AB17:AF17)</f>
-        <v>0.42499999999999999</v>
+        <v>0.44000000000000006</v>
       </c>
       <c r="H23">
         <f>AVERAGE(H17:L17,AG17:AK17)</f>
@@ -5564,15 +5886,15 @@
       </c>
       <c r="M23">
         <f>AVERAGE(M17:Q17,AL17:AP17)</f>
-        <v>0.5</v>
+        <v>0.49999999999999989</v>
       </c>
       <c r="R23">
         <f>AVERAGE(R17:V17,AQ17:AU17)</f>
-        <v>0.375</v>
+        <v>0.34</v>
       </c>
       <c r="W23">
         <f>AVERAGE(W17:AA17,AV17:AZ17)</f>
-        <v>0.42499999999999999</v>
+        <v>0.44000000000000006</v>
       </c>
     </row>
     <row r="25" spans="3:52">
@@ -5581,19 +5903,19 @@
         <v>Amplitude 0</v>
       </c>
       <c r="D25" t="str">
-        <f t="shared" ref="D25:G25" si="14">D4</f>
+        <f t="shared" ref="D25:G25" si="15">D4</f>
         <v>Amplitude 100</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Amplitude 25</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Amplitude 50</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Amplitude 75</v>
       </c>
     </row>
@@ -5603,20 +5925,20 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <f t="shared" ref="D26:G26" si="15">AVERAGE(D17,I17,N17,S17,X17,AC17,AH17,AM17,AR17,AW17)</f>
-        <v>0.82499999999999996</v>
+        <f t="shared" ref="D26:G26" si="16">AVERAGE(D17,I17,N17,S17,X17,AC17,AH17,AM17,AR17,AW17)</f>
+        <v>0.79999999999999993</v>
       </c>
       <c r="E26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.1</v>
       </c>
       <c r="F26">
-        <f t="shared" si="15"/>
-        <v>0.5</v>
+        <f t="shared" si="16"/>
+        <v>0.50000000000000011</v>
       </c>
       <c r="G26">
-        <f t="shared" si="15"/>
-        <v>0.7</v>
+        <f t="shared" si="16"/>
+        <v>0.72</v>
       </c>
     </row>
     <row r="29" spans="3:52">
@@ -5641,7 +5963,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5650,7 +5973,7 @@
   <dimension ref="A1:CX56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AZ46" sqref="AZ46"/>
+      <selection activeCell="AZ48" sqref="AZ48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8624,6 +8947,311 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="9" spans="1:102">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>-1</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>-1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+      <c r="H9">
+        <v>-1</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>-1</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="M9">
+        <v>-1</v>
+      </c>
+      <c r="N9">
+        <v>7</v>
+      </c>
+      <c r="O9">
+        <v>-1</v>
+      </c>
+      <c r="P9">
+        <v>-1</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>-1</v>
+      </c>
+      <c r="S9">
+        <v>11</v>
+      </c>
+      <c r="T9">
+        <v>-1</v>
+      </c>
+      <c r="U9">
+        <v>-1</v>
+      </c>
+      <c r="V9">
+        <v>-1</v>
+      </c>
+      <c r="W9">
+        <v>-1</v>
+      </c>
+      <c r="X9">
+        <v>10</v>
+      </c>
+      <c r="Y9">
+        <v>-1</v>
+      </c>
+      <c r="Z9">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>1</v>
+      </c>
+      <c r="AB9">
+        <v>-1</v>
+      </c>
+      <c r="AC9">
+        <v>-1</v>
+      </c>
+      <c r="AD9">
+        <v>1</v>
+      </c>
+      <c r="AE9">
+        <v>-1</v>
+      </c>
+      <c r="AF9">
+        <v>7</v>
+      </c>
+      <c r="AG9">
+        <v>-1</v>
+      </c>
+      <c r="AH9">
+        <v>4</v>
+      </c>
+      <c r="AI9">
+        <v>-1</v>
+      </c>
+      <c r="AJ9">
+        <v>-1</v>
+      </c>
+      <c r="AK9">
+        <v>-1</v>
+      </c>
+      <c r="AL9">
+        <v>-1</v>
+      </c>
+      <c r="AM9">
+        <v>4</v>
+      </c>
+      <c r="AN9">
+        <v>-1</v>
+      </c>
+      <c r="AO9">
+        <v>8</v>
+      </c>
+      <c r="AP9">
+        <v>1</v>
+      </c>
+      <c r="AQ9">
+        <v>-1</v>
+      </c>
+      <c r="AR9">
+        <v>-1</v>
+      </c>
+      <c r="AS9">
+        <v>-1</v>
+      </c>
+      <c r="AT9">
+        <v>-1</v>
+      </c>
+      <c r="AU9">
+        <v>173</v>
+      </c>
+      <c r="AV9">
+        <v>-1</v>
+      </c>
+      <c r="AW9">
+        <v>-1</v>
+      </c>
+      <c r="AX9">
+        <v>-1</v>
+      </c>
+      <c r="AY9">
+        <v>55</v>
+      </c>
+      <c r="AZ9">
+        <v>11</v>
+      </c>
+      <c r="BA9">
+        <v>-1</v>
+      </c>
+      <c r="BB9">
+        <v>2</v>
+      </c>
+      <c r="BC9">
+        <v>-1</v>
+      </c>
+      <c r="BD9">
+        <v>2</v>
+      </c>
+      <c r="BE9">
+        <v>3</v>
+      </c>
+      <c r="BF9">
+        <v>-1</v>
+      </c>
+      <c r="BG9">
+        <v>0</v>
+      </c>
+      <c r="BH9">
+        <v>-1</v>
+      </c>
+      <c r="BI9">
+        <v>-1</v>
+      </c>
+      <c r="BJ9">
+        <v>0</v>
+      </c>
+      <c r="BK9">
+        <v>-1</v>
+      </c>
+      <c r="BL9">
+        <v>6</v>
+      </c>
+      <c r="BM9">
+        <v>-1</v>
+      </c>
+      <c r="BN9">
+        <v>4</v>
+      </c>
+      <c r="BO9">
+        <v>2</v>
+      </c>
+      <c r="BP9">
+        <v>-1</v>
+      </c>
+      <c r="BQ9">
+        <v>90</v>
+      </c>
+      <c r="BR9">
+        <v>-1</v>
+      </c>
+      <c r="BS9">
+        <v>3</v>
+      </c>
+      <c r="BT9">
+        <v>68</v>
+      </c>
+      <c r="BU9">
+        <v>-1</v>
+      </c>
+      <c r="BV9">
+        <v>5</v>
+      </c>
+      <c r="BW9">
+        <v>190</v>
+      </c>
+      <c r="BX9">
+        <v>-1</v>
+      </c>
+      <c r="BY9">
+        <v>115</v>
+      </c>
+      <c r="BZ9">
+        <v>-1</v>
+      </c>
+      <c r="CA9">
+        <v>4</v>
+      </c>
+      <c r="CB9">
+        <v>-1</v>
+      </c>
+      <c r="CC9">
+        <v>-1</v>
+      </c>
+      <c r="CD9">
+        <v>-1</v>
+      </c>
+      <c r="CE9">
+        <v>-1</v>
+      </c>
+      <c r="CF9">
+        <v>2</v>
+      </c>
+      <c r="CG9">
+        <v>-1</v>
+      </c>
+      <c r="CH9">
+        <v>4</v>
+      </c>
+      <c r="CI9">
+        <v>-1</v>
+      </c>
+      <c r="CJ9">
+        <v>-1</v>
+      </c>
+      <c r="CK9">
+        <v>4</v>
+      </c>
+      <c r="CL9">
+        <v>1</v>
+      </c>
+      <c r="CM9">
+        <v>-1</v>
+      </c>
+      <c r="CN9">
+        <v>4</v>
+      </c>
+      <c r="CO9">
+        <v>-1</v>
+      </c>
+      <c r="CP9">
+        <v>-1</v>
+      </c>
+      <c r="CQ9">
+        <v>-1</v>
+      </c>
+      <c r="CR9">
+        <v>-1</v>
+      </c>
+      <c r="CS9">
+        <v>16</v>
+      </c>
+      <c r="CT9">
+        <v>-1</v>
+      </c>
+      <c r="CU9">
+        <v>9</v>
+      </c>
+      <c r="CV9">
+        <v>-1</v>
+      </c>
+      <c r="CW9">
+        <v>4</v>
+      </c>
+      <c r="CX9">
+        <v>-1</v>
+      </c>
+    </row>
     <row r="22" spans="3:102">
       <c r="C22" t="str">
         <f>IF(C6&gt;=0,C6,"")</f>
@@ -9831,17 +10459,17 @@
       </c>
     </row>
     <row r="25" spans="3:102">
-      <c r="C25">
+      <c r="C25" t="str">
         <f t="shared" ref="C25:BN25" si="6">IF(C9&gt;=0,C9,"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D25">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E25">
+        <v>7</v>
+      </c>
+      <c r="E25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="F25">
         <f t="shared" si="6"/>
@@ -9849,19 +10477,19 @@
       </c>
       <c r="G25">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H25">
+        <v>6</v>
+      </c>
+      <c r="H25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="I25">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J25">
+        <v>4</v>
+      </c>
+      <c r="J25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="K25">
         <f t="shared" si="6"/>
@@ -9869,367 +10497,367 @@
       </c>
       <c r="L25">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M25">
+        <v>2</v>
+      </c>
+      <c r="M25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="N25">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O25">
+        <v>7</v>
+      </c>
+      <c r="O25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P25">
+        <v/>
+      </c>
+      <c r="P25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="Q25">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R25">
+      <c r="R25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="S25">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T25">
+        <v>11</v>
+      </c>
+      <c r="T25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U25">
+        <v/>
+      </c>
+      <c r="U25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V25">
+        <v/>
+      </c>
+      <c r="V25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="W25">
+        <v/>
+      </c>
+      <c r="W25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="X25">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Y25">
+        <v>10</v>
+      </c>
+      <c r="Y25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="Z25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA25">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AB25">
+        <v>1</v>
+      </c>
+      <c r="AB25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AC25">
+        <v/>
+      </c>
+      <c r="AC25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AD25">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AE25">
+        <v>1</v>
+      </c>
+      <c r="AE25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AF25">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AG25">
+        <v>7</v>
+      </c>
+      <c r="AG25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AH25">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI25">
+        <v>4</v>
+      </c>
+      <c r="AI25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AJ25">
+        <v/>
+      </c>
+      <c r="AJ25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AK25">
+        <v/>
+      </c>
+      <c r="AK25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AL25">
+        <v/>
+      </c>
+      <c r="AL25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AM25">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AN25">
+        <v>4</v>
+      </c>
+      <c r="AN25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AO25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AP25">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AQ25">
+        <v>1</v>
+      </c>
+      <c r="AQ25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AR25">
+        <v/>
+      </c>
+      <c r="AR25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AS25">
+        <v/>
+      </c>
+      <c r="AS25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AT25">
+        <v/>
+      </c>
+      <c r="AT25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AU25">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AV25">
+        <v>173</v>
+      </c>
+      <c r="AV25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AW25">
+        <v/>
+      </c>
+      <c r="AW25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AX25">
+        <v/>
+      </c>
+      <c r="AX25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AY25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="AZ25">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="BA25">
+        <v>11</v>
+      </c>
+      <c r="BA25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BB25">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="BC25">
+        <v>2</v>
+      </c>
+      <c r="BC25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BD25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BE25">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="BF25">
+        <v>3</v>
+      </c>
+      <c r="BF25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BG25">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="BH25">
+      <c r="BH25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="BI25">
+        <v/>
+      </c>
+      <c r="BI25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BJ25">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="BK25">
+      <c r="BK25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BL25">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="BM25">
+        <v>6</v>
+      </c>
+      <c r="BM25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BN25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BO25">
         <f t="shared" ref="BO25:CX25" si="7">IF(BO9&gt;=0,BO9,"")</f>
-        <v>0</v>
-      </c>
-      <c r="BP25">
+        <v>2</v>
+      </c>
+      <c r="BP25" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BQ25">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="BR25">
+        <v>90</v>
+      </c>
+      <c r="BR25" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BS25">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BT25">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="BU25">
+        <v>68</v>
+      </c>
+      <c r="BU25" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BV25">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BW25">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="BX25">
+        <v>190</v>
+      </c>
+      <c r="BX25" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BY25">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="BZ25">
+        <v>115</v>
+      </c>
+      <c r="BZ25" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CA25">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="CB25">
+        <v>4</v>
+      </c>
+      <c r="CB25" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="CC25">
+        <v/>
+      </c>
+      <c r="CC25" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="CD25">
+        <v/>
+      </c>
+      <c r="CD25" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="CE25">
+        <v/>
+      </c>
+      <c r="CE25" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CF25">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="CG25">
+        <v>2</v>
+      </c>
+      <c r="CG25" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CH25">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="CI25">
+        <v>4</v>
+      </c>
+      <c r="CI25" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="CJ25">
+        <v/>
+      </c>
+      <c r="CJ25" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CK25">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="CL25">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="CM25">
+        <v>1</v>
+      </c>
+      <c r="CM25" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CN25">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="CO25">
+        <v>4</v>
+      </c>
+      <c r="CO25" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="CP25">
+        <v/>
+      </c>
+      <c r="CP25" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="CQ25">
+        <v/>
+      </c>
+      <c r="CQ25" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="CR25">
+        <v/>
+      </c>
+      <c r="CR25" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CS25">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="CT25">
+        <v>16</v>
+      </c>
+      <c r="CT25" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CU25">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="CV25">
+        <v>9</v>
+      </c>
+      <c r="CV25" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CW25">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="CX25">
+        <v>4</v>
+      </c>
+      <c r="CX25" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="3:102">
@@ -13455,12 +14083,12 @@
     </row>
     <row r="43" spans="3:102">
       <c r="C43" t="e">
-        <f>AVERAGE(C22:C24,BA22)</f>
+        <f>AVERAGE(C22:C25,BA22)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D43">
-        <f t="shared" ref="D43:AZ43" si="24">AVERAGE(D22:D24,BB22)</f>
-        <v>4.25</v>
+        <f t="shared" ref="D43:AZ43" si="24">AVERAGE(D22:D25,BB22)</f>
+        <v>4.8</v>
       </c>
       <c r="E43">
         <f t="shared" si="24"/>
@@ -13468,11 +14096,11 @@
       </c>
       <c r="F43">
         <f t="shared" si="24"/>
-        <v>2.3333333333333335</v>
+        <v>1.75</v>
       </c>
       <c r="G43">
         <f t="shared" si="24"/>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="H43" t="e">
         <f t="shared" si="24"/>
@@ -13480,7 +14108,7 @@
       </c>
       <c r="I43">
         <f t="shared" si="24"/>
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="J43" t="e">
         <f t="shared" si="24"/>
@@ -13488,11 +14116,11 @@
       </c>
       <c r="K43">
         <f t="shared" si="24"/>
-        <v>7.666666666666667</v>
+        <v>5.75</v>
       </c>
       <c r="L43">
         <f t="shared" si="24"/>
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="M43" t="e">
         <f t="shared" si="24"/>
@@ -13500,7 +14128,7 @@
       </c>
       <c r="N43">
         <f t="shared" si="24"/>
-        <v>4</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="O43">
         <f t="shared" si="24"/>
@@ -13512,7 +14140,7 @@
       </c>
       <c r="Q43">
         <f t="shared" si="24"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R43" t="e">
         <f t="shared" si="24"/>
@@ -13520,7 +14148,7 @@
       </c>
       <c r="S43">
         <f t="shared" si="24"/>
-        <v>40.25</v>
+        <v>34.4</v>
       </c>
       <c r="T43" t="e">
         <f t="shared" si="24"/>
@@ -13540,7 +14168,7 @@
       </c>
       <c r="X43">
         <f t="shared" si="24"/>
-        <v>24</v>
+        <v>20.5</v>
       </c>
       <c r="Y43">
         <f t="shared" si="24"/>
@@ -13548,11 +14176,11 @@
       </c>
       <c r="Z43">
         <f t="shared" si="24"/>
-        <v>115</v>
+        <v>77</v>
       </c>
       <c r="AA43">
         <f t="shared" si="24"/>
-        <v>12</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AB43" t="e">
         <f t="shared" si="24"/>
@@ -13562,9 +14190,9 @@
         <f t="shared" si="24"/>
         <v>2.6666666666666665</v>
       </c>
-      <c r="AD43" t="e">
+      <c r="AD43">
         <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="AE43">
         <f t="shared" si="24"/>
@@ -13572,7 +14200,7 @@
       </c>
       <c r="AF43">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AG43" t="e">
         <f t="shared" si="24"/>
@@ -13580,7 +14208,7 @@
       </c>
       <c r="AH43">
         <f t="shared" si="24"/>
-        <v>2.3333333333333335</v>
+        <v>2.75</v>
       </c>
       <c r="AI43" t="e">
         <f t="shared" si="24"/>
@@ -13600,7 +14228,7 @@
       </c>
       <c r="AM43">
         <f t="shared" si="24"/>
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="AN43" t="e">
         <f t="shared" si="24"/>
@@ -13608,11 +14236,11 @@
       </c>
       <c r="AO43">
         <f t="shared" si="24"/>
-        <v>3.6666666666666665</v>
+        <v>4.75</v>
       </c>
       <c r="AP43">
         <f t="shared" si="24"/>
-        <v>163.33333333333334</v>
+        <v>122.75</v>
       </c>
       <c r="AQ43" t="e">
         <f t="shared" si="24"/>
@@ -13632,7 +14260,7 @@
       </c>
       <c r="AU43">
         <f t="shared" si="24"/>
-        <v>187.33333333333334</v>
+        <v>183.75</v>
       </c>
       <c r="AV43" t="e">
         <f t="shared" si="24"/>
@@ -13646,13 +14274,13 @@
         <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AY43" t="e">
+      <c r="AY43">
         <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
+        <v>55</v>
       </c>
       <c r="AZ43">
         <f t="shared" si="24"/>
-        <v>161.66666666666666</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="3:102">
@@ -13662,7 +14290,7 @@
       </c>
       <c r="D44">
         <f t="shared" ref="D44:AZ44" si="25">IF(ISNUMBER(D43),D43,"")</f>
-        <v>4.25</v>
+        <v>4.8</v>
       </c>
       <c r="E44">
         <f t="shared" si="25"/>
@@ -13670,11 +14298,11 @@
       </c>
       <c r="F44">
         <f t="shared" si="25"/>
-        <v>2.3333333333333335</v>
+        <v>1.75</v>
       </c>
       <c r="G44">
         <f t="shared" si="25"/>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="25"/>
@@ -13682,7 +14310,7 @@
       </c>
       <c r="I44">
         <f t="shared" si="25"/>
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="J44" t="str">
         <f t="shared" si="25"/>
@@ -13690,11 +14318,11 @@
       </c>
       <c r="K44">
         <f t="shared" si="25"/>
-        <v>7.666666666666667</v>
+        <v>5.75</v>
       </c>
       <c r="L44">
         <f t="shared" si="25"/>
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="M44" t="str">
         <f t="shared" si="25"/>
@@ -13702,7 +14330,7 @@
       </c>
       <c r="N44">
         <f t="shared" si="25"/>
-        <v>4</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="O44">
         <f t="shared" si="25"/>
@@ -13714,7 +14342,7 @@
       </c>
       <c r="Q44">
         <f t="shared" si="25"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R44" t="str">
         <f t="shared" si="25"/>
@@ -13722,7 +14350,7 @@
       </c>
       <c r="S44">
         <f t="shared" si="25"/>
-        <v>40.25</v>
+        <v>34.4</v>
       </c>
       <c r="T44" t="str">
         <f t="shared" si="25"/>
@@ -13742,7 +14370,7 @@
       </c>
       <c r="X44">
         <f t="shared" si="25"/>
-        <v>24</v>
+        <v>20.5</v>
       </c>
       <c r="Y44">
         <f t="shared" si="25"/>
@@ -13750,11 +14378,11 @@
       </c>
       <c r="Z44">
         <f t="shared" si="25"/>
-        <v>115</v>
+        <v>77</v>
       </c>
       <c r="AA44">
         <f t="shared" si="25"/>
-        <v>12</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AB44" t="str">
         <f t="shared" si="25"/>
@@ -13764,9 +14392,9 @@
         <f t="shared" si="25"/>
         <v>2.6666666666666665</v>
       </c>
-      <c r="AD44" t="str">
+      <c r="AD44">
         <f t="shared" si="25"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AE44">
         <f t="shared" si="25"/>
@@ -13774,7 +14402,7 @@
       </c>
       <c r="AF44">
         <f t="shared" si="25"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AG44" t="str">
         <f t="shared" si="25"/>
@@ -13782,7 +14410,7 @@
       </c>
       <c r="AH44">
         <f t="shared" si="25"/>
-        <v>2.3333333333333335</v>
+        <v>2.75</v>
       </c>
       <c r="AI44" t="str">
         <f t="shared" si="25"/>
@@ -13802,7 +14430,7 @@
       </c>
       <c r="AM44">
         <f t="shared" si="25"/>
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="AN44" t="str">
         <f t="shared" si="25"/>
@@ -13810,11 +14438,11 @@
       </c>
       <c r="AO44">
         <f t="shared" si="25"/>
-        <v>3.6666666666666665</v>
+        <v>4.75</v>
       </c>
       <c r="AP44">
         <f t="shared" si="25"/>
-        <v>163.33333333333334</v>
+        <v>122.75</v>
       </c>
       <c r="AQ44" t="str">
         <f t="shared" si="25"/>
@@ -13834,7 +14462,7 @@
       </c>
       <c r="AU44">
         <f t="shared" si="25"/>
-        <v>187.33333333333334</v>
+        <v>183.75</v>
       </c>
       <c r="AV44" t="str">
         <f t="shared" si="25"/>
@@ -13848,13 +14476,13 @@
         <f t="shared" si="25"/>
         <v/>
       </c>
-      <c r="AY44" t="str">
+      <c r="AY44">
         <f t="shared" si="25"/>
-        <v/>
+        <v>55</v>
       </c>
       <c r="AZ44">
         <f t="shared" si="25"/>
-        <v>161.66666666666666</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48" spans="3:102">
@@ -13868,11 +14496,11 @@
     <row r="49" spans="3:23">
       <c r="C49">
         <f>AVERAGE(C44:AA44)</f>
-        <v>19.583333333333332</v>
+        <v>16.725000000000001</v>
       </c>
       <c r="D49">
         <f>AVERAGE(AB44:AZ44)</f>
-        <v>84.095238095238102</v>
+        <v>71.75</v>
       </c>
     </row>
     <row r="51" spans="3:23">
@@ -13900,23 +14528,23 @@
     <row r="52" spans="3:23">
       <c r="C52">
         <f>AVERAGE(C44:G44,AB44:AF44)</f>
-        <v>5.8214285714285712</v>
+        <v>5.6520833333333336</v>
       </c>
       <c r="H52">
         <f>AVERAGE(H44:L44,AG44:AK44)</f>
-        <v>5.25</v>
+        <v>4.9916666666666663</v>
       </c>
       <c r="M52">
         <f>AVERAGE(M44:Q44,AL44:AP44)</f>
-        <v>32.80952380952381</v>
+        <v>25.966666666666665</v>
       </c>
       <c r="R52">
         <f>AVERAGE(R44:V44,AQ44:AU44)</f>
-        <v>134.56944444444446</v>
+        <v>132.99722222222223</v>
       </c>
       <c r="W52">
         <f>AVERAGE(W44:AA44,AV44:AZ44)</f>
-        <v>70.083333333333329</v>
+        <v>56.304761904761904</v>
       </c>
     </row>
     <row r="55" spans="3:23">
@@ -13948,19 +14576,19 @@
       </c>
       <c r="D56">
         <f>AVERAGE(D44,I44,N44,S44,X44,AC44,AH44,AM44,AR44,AW44)</f>
-        <v>32.733333333333334</v>
+        <v>31.175000000000001</v>
       </c>
       <c r="E56">
         <f>AVERAGE(E44,J44,O44,T44,Y44,AD44,AI44,AN44,AS44,AX44)</f>
-        <v>10.833333333333334</v>
+        <v>8.375</v>
       </c>
       <c r="F56">
         <f>AVERAGE(F44,K44,P44,U44,Z44,AE44,AJ44,AO44,AT44,AY44)</f>
-        <v>68.648148148148152</v>
+        <v>63.341666666666676</v>
       </c>
       <c r="G56">
         <f>AVERAGE(G44,L44,Q44,V44,AA44,AF44,AK44,AP44,AU44,AZ44)</f>
-        <v>55.216666666666661</v>
+        <v>47.038333333333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pilot 1 - User 5.
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -936,33 +936,33 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.52</c:v>
+                  <c:v>0.4920000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32800000000000007</c:v>
+                  <c:v>0.33199999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="50313856"/>
-        <c:axId val="50323840"/>
+        <c:axId val="49417216"/>
+        <c:axId val="49419008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50313856"/>
+        <c:axId val="49417216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50323840"/>
+        <c:crossAx val="49419008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50323840"/>
+        <c:axId val="49419008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -972,7 +972,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50313856"/>
+        <c:crossAx val="49417216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -981,7 +981,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1029,42 +1029,42 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.44000000000000006</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.4</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.49999999999999989</c:v>
+                  <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.34</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.44000000000000006</c:v>
+                  <c:v>0.41999999999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="50203648"/>
-        <c:axId val="50217728"/>
+        <c:axId val="49438080"/>
+        <c:axId val="49456256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50203648"/>
+        <c:axId val="49438080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50217728"/>
+        <c:crossAx val="49456256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50217728"/>
+        <c:axId val="49456256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1074,7 +1074,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50203648"/>
+        <c:crossAx val="49438080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1083,7 +1083,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1134,39 +1134,39 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.79999999999999993</c:v>
+                  <c:v>0.81000000000000016</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.50000000000000011</c:v>
+                  <c:v>0.45999999999999985</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.72</c:v>
+                  <c:v>0.69000000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="50228608"/>
-        <c:axId val="50250880"/>
+        <c:axId val="50204672"/>
+        <c:axId val="50206208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50228608"/>
+        <c:axId val="50204672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50250880"/>
+        <c:crossAx val="50206208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50250880"/>
+        <c:axId val="50206208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1174,7 +1174,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50228608"/>
+        <c:crossAx val="50204672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1183,7 +1183,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1369,16 +1369,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1387,10 +1387,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.8</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.8</c:v>
@@ -1408,13 +1408,13 @@
                   <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.8</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
@@ -1429,28 +1429,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.8</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.4</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.6</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.6</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.2</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>0.4</c:v>
@@ -1465,78 +1465,78 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.4</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.2</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.8</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.8</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.8</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.4</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.8</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.6</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.2</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.8</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="50352128"/>
-        <c:axId val="50353664"/>
+        <c:axId val="50229632"/>
+        <c:axId val="50231168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50352128"/>
+        <c:axId val="50229632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50353664"/>
+        <c:crossAx val="50231168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50353664"/>
+        <c:axId val="50231168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1546,7 +1546,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50352128"/>
+        <c:crossAx val="50229632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1555,7 +1555,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1603,24 +1603,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="50377088"/>
-        <c:axId val="50378624"/>
+        <c:axId val="50279168"/>
+        <c:axId val="50280704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50377088"/>
+        <c:axId val="50279168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50378624"/>
+        <c:crossAx val="50280704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50378624"/>
+        <c:axId val="50280704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1630,7 +1630,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50377088"/>
+        <c:crossAx val="50279168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1639,7 +1639,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1678,33 +1678,33 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>16.725000000000001</c:v>
+                  <c:v>23.43398078529658</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>71.75</c:v>
+                  <c:v>87.409477124183013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="50803840"/>
-        <c:axId val="50805376"/>
+        <c:axId val="50828800"/>
+        <c:axId val="50830336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50803840"/>
+        <c:axId val="50828800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50805376"/>
+        <c:crossAx val="50830336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50805376"/>
+        <c:axId val="50830336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1712,7 +1712,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50803840"/>
+        <c:crossAx val="50828800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1721,7 +1721,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1769,42 +1769,42 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5.6520833333333336</c:v>
+                  <c:v>12.638888888888889</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9916666666666663</c:v>
+                  <c:v>36.323979591836732</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.966666666666665</c:v>
+                  <c:v>12.820833333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>132.99722222222223</c:v>
+                  <c:v>140.63425925925927</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>56.304761904761904</c:v>
+                  <c:v>89.922222222222217</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="50832896"/>
-        <c:axId val="50834432"/>
+        <c:axId val="50337664"/>
+        <c:axId val="50339200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50832896"/>
+        <c:axId val="50337664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50834432"/>
+        <c:crossAx val="50339200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50834432"/>
+        <c:axId val="50339200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1812,7 +1812,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50832896"/>
+        <c:crossAx val="50337664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1821,7 +1821,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1872,39 +1872,39 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.175000000000001</c:v>
+                  <c:v>40.105000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.375</c:v>
+                  <c:v>16.333333333333332</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>63.341666666666676</c:v>
+                  <c:v>72.539285714285725</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>47.038333333333334</c:v>
+                  <c:v>70.676388888888894</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="51058176"/>
-        <c:axId val="51059712"/>
+        <c:axId val="50349952"/>
+        <c:axId val="50351488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="51058176"/>
+        <c:axId val="50349952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51059712"/>
+        <c:crossAx val="50351488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51059712"/>
+        <c:axId val="50351488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1912,7 +1912,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51058176"/>
+        <c:crossAx val="50349952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1921,7 +1921,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2464,8 +2464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DA30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T34" sqref="T34"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="CS36" sqref="CS36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5006,7 +5006,7 @@
         <v>1</v>
       </c>
       <c r="DA7" s="1">
-        <f t="shared" ref="DA7:DA9" si="13">SUM(C7:CX7)</f>
+        <f t="shared" ref="DA7:DA10" si="13">SUM(C7:CX7)</f>
         <v>52</v>
       </c>
     </row>
@@ -5628,6 +5628,315 @@
         <v>44</v>
       </c>
     </row>
+    <row r="10" spans="1:105">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>1</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>1</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>1</v>
+      </c>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10">
+        <v>1</v>
+      </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+      <c r="AJ10">
+        <v>0</v>
+      </c>
+      <c r="AK10">
+        <v>0</v>
+      </c>
+      <c r="AL10">
+        <v>0</v>
+      </c>
+      <c r="AM10">
+        <v>1</v>
+      </c>
+      <c r="AN10">
+        <v>0</v>
+      </c>
+      <c r="AO10">
+        <v>1</v>
+      </c>
+      <c r="AP10">
+        <v>1</v>
+      </c>
+      <c r="AQ10">
+        <v>0</v>
+      </c>
+      <c r="AR10">
+        <v>0</v>
+      </c>
+      <c r="AS10">
+        <v>0</v>
+      </c>
+      <c r="AT10">
+        <v>0</v>
+      </c>
+      <c r="AU10">
+        <v>1</v>
+      </c>
+      <c r="AV10">
+        <v>0</v>
+      </c>
+      <c r="AW10">
+        <v>1</v>
+      </c>
+      <c r="AX10">
+        <v>0</v>
+      </c>
+      <c r="AY10">
+        <v>0</v>
+      </c>
+      <c r="AZ10">
+        <v>0</v>
+      </c>
+      <c r="BA10">
+        <v>0</v>
+      </c>
+      <c r="BB10">
+        <v>1</v>
+      </c>
+      <c r="BC10">
+        <v>0</v>
+      </c>
+      <c r="BD10">
+        <v>0</v>
+      </c>
+      <c r="BE10">
+        <v>1</v>
+      </c>
+      <c r="BF10">
+        <v>0</v>
+      </c>
+      <c r="BG10">
+        <v>1</v>
+      </c>
+      <c r="BH10">
+        <v>1</v>
+      </c>
+      <c r="BI10">
+        <v>0</v>
+      </c>
+      <c r="BJ10">
+        <v>1</v>
+      </c>
+      <c r="BK10">
+        <v>0</v>
+      </c>
+      <c r="BL10">
+        <v>1</v>
+      </c>
+      <c r="BM10">
+        <v>0</v>
+      </c>
+      <c r="BN10">
+        <v>0</v>
+      </c>
+      <c r="BO10">
+        <v>1</v>
+      </c>
+      <c r="BP10">
+        <v>0</v>
+      </c>
+      <c r="BQ10">
+        <v>1</v>
+      </c>
+      <c r="BR10">
+        <v>0</v>
+      </c>
+      <c r="BS10">
+        <v>0</v>
+      </c>
+      <c r="BT10">
+        <v>0</v>
+      </c>
+      <c r="BU10">
+        <v>0</v>
+      </c>
+      <c r="BV10">
+        <v>1</v>
+      </c>
+      <c r="BW10">
+        <v>0</v>
+      </c>
+      <c r="BX10">
+        <v>0</v>
+      </c>
+      <c r="BY10">
+        <v>1</v>
+      </c>
+      <c r="BZ10">
+        <v>0</v>
+      </c>
+      <c r="CA10">
+        <v>1</v>
+      </c>
+      <c r="CB10">
+        <v>0</v>
+      </c>
+      <c r="CC10">
+        <v>1</v>
+      </c>
+      <c r="CD10">
+        <v>0</v>
+      </c>
+      <c r="CE10">
+        <v>0</v>
+      </c>
+      <c r="CF10">
+        <v>1</v>
+      </c>
+      <c r="CG10">
+        <v>0</v>
+      </c>
+      <c r="CH10">
+        <v>0</v>
+      </c>
+      <c r="CI10">
+        <v>1</v>
+      </c>
+      <c r="CJ10">
+        <v>0</v>
+      </c>
+      <c r="CK10">
+        <v>1</v>
+      </c>
+      <c r="CL10">
+        <v>0</v>
+      </c>
+      <c r="CM10">
+        <v>0</v>
+      </c>
+      <c r="CN10">
+        <v>1</v>
+      </c>
+      <c r="CO10">
+        <v>0</v>
+      </c>
+      <c r="CP10">
+        <v>0</v>
+      </c>
+      <c r="CQ10">
+        <v>0</v>
+      </c>
+      <c r="CR10">
+        <v>0</v>
+      </c>
+      <c r="CS10">
+        <v>0</v>
+      </c>
+      <c r="CT10">
+        <v>0</v>
+      </c>
+      <c r="CU10">
+        <v>1</v>
+      </c>
+      <c r="CV10">
+        <v>0</v>
+      </c>
+      <c r="CW10">
+        <v>1</v>
+      </c>
+      <c r="CX10">
+        <v>1</v>
+      </c>
+      <c r="DA10" s="1">
+        <f t="shared" si="13"/>
+        <v>36</v>
+      </c>
+    </row>
     <row r="16" spans="1:105">
       <c r="C16" t="s">
         <v>31</v>
@@ -5635,24 +5944,24 @@
     </row>
     <row r="17" spans="3:52">
       <c r="C17">
-        <f>AVERAGE(C6:C14,BA6)</f>
+        <f>AVERAGE(C6:C14,BA6:BA15)</f>
         <v>0</v>
       </c>
       <c r="D17">
-        <f t="shared" ref="D17:AZ17" si="14">AVERAGE(D6:D14,BB6)</f>
-        <v>1</v>
+        <f t="shared" ref="D17:AZ17" si="14">AVERAGE(D6:D14,BB6:BB15)</f>
+        <v>0.9</v>
       </c>
       <c r="E17">
         <f t="shared" si="14"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F17">
         <f t="shared" si="14"/>
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="G17">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="H17">
         <f t="shared" si="14"/>
@@ -5664,11 +5973,11 @@
       </c>
       <c r="J17">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="K17">
         <f t="shared" si="14"/>
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="L17">
         <f t="shared" si="14"/>
@@ -5692,7 +6001,7 @@
       </c>
       <c r="Q17">
         <f t="shared" si="14"/>
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="R17">
         <f t="shared" si="14"/>
@@ -5700,7 +6009,7 @@
       </c>
       <c r="S17">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="T17">
         <f t="shared" si="14"/>
@@ -5720,19 +6029,19 @@
       </c>
       <c r="X17">
         <f t="shared" si="14"/>
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="Y17">
         <f t="shared" si="14"/>
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="Z17">
         <f t="shared" si="14"/>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="AA17">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AB17">
         <f t="shared" si="14"/>
@@ -5740,15 +6049,15 @@
       </c>
       <c r="AC17">
         <f t="shared" si="14"/>
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="AD17">
         <f t="shared" si="14"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="AE17">
         <f t="shared" si="14"/>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="AF17">
         <f t="shared" si="14"/>
@@ -5768,11 +6077,11 @@
       </c>
       <c r="AJ17">
         <f t="shared" si="14"/>
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="AK17">
         <f t="shared" si="14"/>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="AL17">
         <f t="shared" si="14"/>
@@ -5780,19 +6089,19 @@
       </c>
       <c r="AM17">
         <f t="shared" si="14"/>
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="AN17">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AO17">
         <f t="shared" si="14"/>
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="AP17">
         <f t="shared" si="14"/>
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="AQ17">
         <f t="shared" si="14"/>
@@ -5800,7 +6109,7 @@
       </c>
       <c r="AR17">
         <f t="shared" si="14"/>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AS17">
         <f t="shared" si="14"/>
@@ -5808,11 +6117,11 @@
       </c>
       <c r="AT17">
         <f t="shared" si="14"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="AU17">
         <f t="shared" si="14"/>
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="AV17">
         <f t="shared" si="14"/>
@@ -5820,7 +6129,7 @@
       </c>
       <c r="AW17">
         <f t="shared" si="14"/>
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="AX17">
         <f t="shared" si="14"/>
@@ -5828,11 +6137,11 @@
       </c>
       <c r="AY17">
         <f t="shared" si="14"/>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="AZ17">
         <f t="shared" si="14"/>
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="19" spans="3:52">
@@ -5846,11 +6155,11 @@
     <row r="20" spans="3:52">
       <c r="C20">
         <f>AVERAGE(C17:AA17)</f>
-        <v>0.52</v>
+        <v>0.4920000000000001</v>
       </c>
       <c r="D20">
         <f>AVERAGE(AB17:AZ17)</f>
-        <v>0.32800000000000007</v>
+        <v>0.33199999999999996</v>
       </c>
     </row>
     <row r="22" spans="3:52">
@@ -5878,23 +6187,23 @@
     <row r="23" spans="3:52">
       <c r="C23">
         <f>AVERAGE(C17:G17,AB17:AF17)</f>
-        <v>0.44000000000000006</v>
+        <v>0.4</v>
       </c>
       <c r="H23">
         <f>AVERAGE(H17:L17,AG17:AK17)</f>
-        <v>0.4</v>
+        <v>0.44000000000000006</v>
       </c>
       <c r="M23">
         <f>AVERAGE(M17:Q17,AL17:AP17)</f>
-        <v>0.49999999999999989</v>
+        <v>0.52</v>
       </c>
       <c r="R23">
         <f>AVERAGE(R17:V17,AQ17:AU17)</f>
-        <v>0.34</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="W23">
         <f>AVERAGE(W17:AA17,AV17:AZ17)</f>
-        <v>0.44000000000000006</v>
+        <v>0.41999999999999993</v>
       </c>
     </row>
     <row r="25" spans="3:52">
@@ -5926,7 +6235,7 @@
       </c>
       <c r="D26">
         <f t="shared" ref="D26:G26" si="16">AVERAGE(D17,I17,N17,S17,X17,AC17,AH17,AM17,AR17,AW17)</f>
-        <v>0.79999999999999993</v>
+        <v>0.81000000000000016</v>
       </c>
       <c r="E26">
         <f t="shared" si="16"/>
@@ -5934,11 +6243,11 @@
       </c>
       <c r="F26">
         <f t="shared" si="16"/>
-        <v>0.50000000000000011</v>
+        <v>0.45999999999999985</v>
       </c>
       <c r="G26">
         <f t="shared" si="16"/>
-        <v>0.72</v>
+        <v>0.69000000000000006</v>
       </c>
     </row>
     <row r="29" spans="3:52">
@@ -5973,7 +6282,7 @@
   <dimension ref="A1:CX56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AZ48" sqref="AZ48"/>
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9252,6 +9561,311 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="10" spans="1:102">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>-1</v>
+      </c>
+      <c r="D10">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>-1</v>
+      </c>
+      <c r="F10">
+        <v>-1</v>
+      </c>
+      <c r="G10">
+        <v>-1</v>
+      </c>
+      <c r="H10">
+        <v>-1</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>6</v>
+      </c>
+      <c r="K10">
+        <v>5</v>
+      </c>
+      <c r="L10">
+        <v>-1</v>
+      </c>
+      <c r="M10">
+        <v>-1</v>
+      </c>
+      <c r="N10">
+        <v>5</v>
+      </c>
+      <c r="O10">
+        <v>-1</v>
+      </c>
+      <c r="P10">
+        <v>3</v>
+      </c>
+      <c r="Q10">
+        <v>3</v>
+      </c>
+      <c r="R10">
+        <v>-1</v>
+      </c>
+      <c r="S10">
+        <v>-1</v>
+      </c>
+      <c r="T10">
+        <v>-1</v>
+      </c>
+      <c r="U10">
+        <v>-1</v>
+      </c>
+      <c r="V10">
+        <v>7</v>
+      </c>
+      <c r="W10">
+        <v>-1</v>
+      </c>
+      <c r="X10">
+        <v>11</v>
+      </c>
+      <c r="Y10">
+        <v>-1</v>
+      </c>
+      <c r="Z10">
+        <v>-1</v>
+      </c>
+      <c r="AA10">
+        <v>-1</v>
+      </c>
+      <c r="AB10">
+        <v>-1</v>
+      </c>
+      <c r="AC10">
+        <v>2</v>
+      </c>
+      <c r="AD10">
+        <v>-1</v>
+      </c>
+      <c r="AE10">
+        <v>-1</v>
+      </c>
+      <c r="AF10">
+        <v>7</v>
+      </c>
+      <c r="AG10">
+        <v>-1</v>
+      </c>
+      <c r="AH10">
+        <v>1</v>
+      </c>
+      <c r="AI10">
+        <v>-1</v>
+      </c>
+      <c r="AJ10">
+        <v>-1</v>
+      </c>
+      <c r="AK10">
+        <v>-1</v>
+      </c>
+      <c r="AL10">
+        <v>-1</v>
+      </c>
+      <c r="AM10">
+        <v>3</v>
+      </c>
+      <c r="AN10">
+        <v>-1</v>
+      </c>
+      <c r="AO10">
+        <v>6</v>
+      </c>
+      <c r="AP10">
+        <v>5</v>
+      </c>
+      <c r="AQ10">
+        <v>-1</v>
+      </c>
+      <c r="AR10">
+        <v>-1</v>
+      </c>
+      <c r="AS10">
+        <v>-1</v>
+      </c>
+      <c r="AT10">
+        <v>-1</v>
+      </c>
+      <c r="AU10">
+        <v>332</v>
+      </c>
+      <c r="AV10">
+        <v>-1</v>
+      </c>
+      <c r="AW10">
+        <v>116</v>
+      </c>
+      <c r="AX10">
+        <v>-1</v>
+      </c>
+      <c r="AY10">
+        <v>-1</v>
+      </c>
+      <c r="AZ10">
+        <v>-1</v>
+      </c>
+      <c r="BA10">
+        <v>-1</v>
+      </c>
+      <c r="BB10">
+        <v>11</v>
+      </c>
+      <c r="BC10">
+        <v>-1</v>
+      </c>
+      <c r="BD10">
+        <v>-1</v>
+      </c>
+      <c r="BE10">
+        <v>4</v>
+      </c>
+      <c r="BF10">
+        <v>-1</v>
+      </c>
+      <c r="BG10">
+        <v>2</v>
+      </c>
+      <c r="BH10">
+        <v>3</v>
+      </c>
+      <c r="BI10">
+        <v>-1</v>
+      </c>
+      <c r="BJ10">
+        <v>6</v>
+      </c>
+      <c r="BK10">
+        <v>-1</v>
+      </c>
+      <c r="BL10">
+        <v>5</v>
+      </c>
+      <c r="BM10">
+        <v>-1</v>
+      </c>
+      <c r="BN10">
+        <v>-1</v>
+      </c>
+      <c r="BO10">
+        <v>4</v>
+      </c>
+      <c r="BP10">
+        <v>-1</v>
+      </c>
+      <c r="BQ10">
+        <v>336</v>
+      </c>
+      <c r="BR10">
+        <v>-1</v>
+      </c>
+      <c r="BS10">
+        <v>-1</v>
+      </c>
+      <c r="BT10">
+        <v>-1</v>
+      </c>
+      <c r="BU10">
+        <v>-1</v>
+      </c>
+      <c r="BV10">
+        <v>5</v>
+      </c>
+      <c r="BW10">
+        <v>-1</v>
+      </c>
+      <c r="BX10">
+        <v>-1</v>
+      </c>
+      <c r="BY10">
+        <v>8</v>
+      </c>
+      <c r="BZ10">
+        <v>-1</v>
+      </c>
+      <c r="CA10">
+        <v>9</v>
+      </c>
+      <c r="CB10">
+        <v>-1</v>
+      </c>
+      <c r="CC10">
+        <v>163</v>
+      </c>
+      <c r="CD10">
+        <v>-1</v>
+      </c>
+      <c r="CE10">
+        <v>-1</v>
+      </c>
+      <c r="CF10">
+        <v>1</v>
+      </c>
+      <c r="CG10">
+        <v>-1</v>
+      </c>
+      <c r="CH10">
+        <v>-1</v>
+      </c>
+      <c r="CI10">
+        <v>3</v>
+      </c>
+      <c r="CJ10">
+        <v>-1</v>
+      </c>
+      <c r="CK10">
+        <v>2</v>
+      </c>
+      <c r="CL10">
+        <v>-1</v>
+      </c>
+      <c r="CM10">
+        <v>-1</v>
+      </c>
+      <c r="CN10">
+        <v>11</v>
+      </c>
+      <c r="CO10">
+        <v>-1</v>
+      </c>
+      <c r="CP10">
+        <v>-1</v>
+      </c>
+      <c r="CQ10">
+        <v>-1</v>
+      </c>
+      <c r="CR10">
+        <v>-1</v>
+      </c>
+      <c r="CS10">
+        <v>-1</v>
+      </c>
+      <c r="CT10">
+        <v>-1</v>
+      </c>
+      <c r="CU10">
+        <v>289</v>
+      </c>
+      <c r="CV10">
+        <v>-1</v>
+      </c>
+      <c r="CW10">
+        <v>33</v>
+      </c>
+      <c r="CX10">
+        <v>150</v>
+      </c>
+    </row>
     <row r="22" spans="3:102">
       <c r="C22" t="str">
         <f>IF(C6&gt;=0,C6,"")</f>
@@ -10861,405 +11475,405 @@
       </c>
     </row>
     <row r="26" spans="3:102">
-      <c r="C26">
+      <c r="C26" t="str">
         <f t="shared" ref="C26:BN26" si="8">IF(C10&gt;=0,C10,"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D26">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="E26">
+        <v>11</v>
+      </c>
+      <c r="E26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="F26">
+        <v/>
+      </c>
+      <c r="F26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G26">
+        <v/>
+      </c>
+      <c r="G26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H26">
+        <v/>
+      </c>
+      <c r="H26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="I26">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J26">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K26">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="L26">
+        <v>5</v>
+      </c>
+      <c r="L26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="M26">
+        <v/>
+      </c>
+      <c r="M26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="N26">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="O26">
+        <v>5</v>
+      </c>
+      <c r="O26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="P26">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q26">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="R26">
+        <v>3</v>
+      </c>
+      <c r="R26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="S26">
+        <v/>
+      </c>
+      <c r="S26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="T26">
+        <v/>
+      </c>
+      <c r="T26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U26">
+        <v/>
+      </c>
+      <c r="U26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="V26">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="W26">
+        <v>7</v>
+      </c>
+      <c r="W26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="X26">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Y26">
+        <v>11</v>
+      </c>
+      <c r="Y26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z26">
+        <v/>
+      </c>
+      <c r="Z26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AA26">
+        <v/>
+      </c>
+      <c r="AA26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AB26">
+        <v/>
+      </c>
+      <c r="AB26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AC26">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AD26">
+        <v>2</v>
+      </c>
+      <c r="AD26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AE26">
+        <v/>
+      </c>
+      <c r="AE26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AF26">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AG26">
+        <v>7</v>
+      </c>
+      <c r="AG26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AH26">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AI26">
+        <v>1</v>
+      </c>
+      <c r="AI26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AJ26">
+        <v/>
+      </c>
+      <c r="AJ26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AK26">
+        <v/>
+      </c>
+      <c r="AK26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AL26">
+        <v/>
+      </c>
+      <c r="AL26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AM26">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AN26">
+        <v>3</v>
+      </c>
+      <c r="AN26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AO26">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AP26">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AQ26">
+        <v>5</v>
+      </c>
+      <c r="AQ26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AR26">
+        <v/>
+      </c>
+      <c r="AR26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AS26">
+        <v/>
+      </c>
+      <c r="AS26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AT26">
+        <v/>
+      </c>
+      <c r="AT26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AU26">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AV26">
+        <v>332</v>
+      </c>
+      <c r="AV26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AW26">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AX26">
+        <v>116</v>
+      </c>
+      <c r="AX26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AY26">
+        <v/>
+      </c>
+      <c r="AY26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AZ26">
+        <v/>
+      </c>
+      <c r="AZ26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="BA26">
+        <v/>
+      </c>
+      <c r="BA26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BB26">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="BC26">
+        <v>11</v>
+      </c>
+      <c r="BC26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="BD26">
+        <v/>
+      </c>
+      <c r="BD26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BE26">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="BF26">
+        <v>4</v>
+      </c>
+      <c r="BF26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BG26">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BH26">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="BI26">
+        <v>3</v>
+      </c>
+      <c r="BI26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BJ26">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="BK26">
+        <v>6</v>
+      </c>
+      <c r="BK26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BL26">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="BM26">
+        <v>5</v>
+      </c>
+      <c r="BM26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="BN26">
+        <v/>
+      </c>
+      <c r="BN26" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BO26">
         <f t="shared" ref="BO26:CX26" si="9">IF(BO10&gt;=0,BO10,"")</f>
-        <v>0</v>
-      </c>
-      <c r="BP26">
+        <v>4</v>
+      </c>
+      <c r="BP26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BQ26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="BR26">
+        <v>336</v>
+      </c>
+      <c r="BR26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="BS26">
+        <v/>
+      </c>
+      <c r="BS26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="BT26">
+        <v/>
+      </c>
+      <c r="BT26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="BU26">
+        <v/>
+      </c>
+      <c r="BU26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BV26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="BW26">
+        <v>5</v>
+      </c>
+      <c r="BW26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="BX26">
+        <v/>
+      </c>
+      <c r="BX26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BY26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="BZ26">
+        <v>8</v>
+      </c>
+      <c r="BZ26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CA26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="CB26">
+        <v>9</v>
+      </c>
+      <c r="CB26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CC26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="CD26">
+        <v>163</v>
+      </c>
+      <c r="CD26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="CE26">
+        <v/>
+      </c>
+      <c r="CE26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CF26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="CG26">
+        <v>1</v>
+      </c>
+      <c r="CG26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="CH26">
+        <v/>
+      </c>
+      <c r="CH26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CI26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="CJ26">
+        <v>3</v>
+      </c>
+      <c r="CJ26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CK26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="CL26">
+        <v>2</v>
+      </c>
+      <c r="CL26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="CM26">
+        <v/>
+      </c>
+      <c r="CM26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CN26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="CO26">
+        <v>11</v>
+      </c>
+      <c r="CO26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="CP26">
+        <v/>
+      </c>
+      <c r="CP26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="CQ26">
+        <v/>
+      </c>
+      <c r="CQ26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="CR26">
+        <v/>
+      </c>
+      <c r="CR26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="CS26">
+        <v/>
+      </c>
+      <c r="CS26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="CT26">
+        <v/>
+      </c>
+      <c r="CT26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CU26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="CV26">
+        <v>289</v>
+      </c>
+      <c r="CV26" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CW26">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="CX26">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="3:102">
@@ -14083,12 +14697,12 @@
     </row>
     <row r="43" spans="3:102">
       <c r="C43" t="e">
-        <f>AVERAGE(C22:C25,BA22)</f>
+        <f>AVERAGE(C22:C26,BA22:BA26)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D43">
-        <f t="shared" ref="D43:AZ43" si="24">AVERAGE(D22:D25,BB22)</f>
-        <v>4.8</v>
+        <f t="shared" ref="D43:AZ43" si="24">AVERAGE(D22:D26,BB22:BB26)</f>
+        <v>6.1111111111111107</v>
       </c>
       <c r="E43">
         <f t="shared" si="24"/>
@@ -14096,11 +14710,11 @@
       </c>
       <c r="F43">
         <f t="shared" si="24"/>
-        <v>1.75</v>
+        <v>3</v>
       </c>
       <c r="G43">
         <f t="shared" si="24"/>
-        <v>4</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="H43" t="e">
         <f t="shared" si="24"/>
@@ -14108,19 +14722,19 @@
       </c>
       <c r="I43">
         <f t="shared" si="24"/>
-        <v>3.2</v>
-      </c>
-      <c r="J43" t="e">
+        <v>3.4</v>
+      </c>
+      <c r="J43">
         <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
+        <v>4.5</v>
       </c>
       <c r="K43">
         <f t="shared" si="24"/>
-        <v>5.75</v>
+        <v>6.1428571428571432</v>
       </c>
       <c r="L43">
         <f t="shared" si="24"/>
-        <v>2.75</v>
+        <v>2.875</v>
       </c>
       <c r="M43" t="e">
         <f t="shared" si="24"/>
@@ -14128,19 +14742,19 @@
       </c>
       <c r="N43">
         <f t="shared" si="24"/>
-        <v>4.5999999999999996</v>
+        <v>5.9</v>
       </c>
       <c r="O43">
         <f t="shared" si="24"/>
-        <v>11</v>
+        <v>7.5</v>
       </c>
       <c r="P43">
         <f t="shared" si="24"/>
-        <v>7.666666666666667</v>
+        <v>6.833333333333333</v>
       </c>
       <c r="Q43">
         <f t="shared" si="24"/>
-        <v>3</v>
+        <v>3.5555555555555554</v>
       </c>
       <c r="R43" t="e">
         <f t="shared" si="24"/>
@@ -14148,7 +14762,7 @@
       </c>
       <c r="S43">
         <f t="shared" si="24"/>
-        <v>34.4</v>
+        <v>105.22222222222223</v>
       </c>
       <c r="T43" t="e">
         <f t="shared" si="24"/>
@@ -14156,11 +14770,11 @@
       </c>
       <c r="U43">
         <f t="shared" si="24"/>
-        <v>86</v>
+        <v>44.75</v>
       </c>
       <c r="V43">
         <f t="shared" si="24"/>
-        <v>3.3333333333333335</v>
+        <v>22.833333333333332</v>
       </c>
       <c r="W43" t="e">
         <f t="shared" si="24"/>
@@ -14168,19 +14782,19 @@
       </c>
       <c r="X43">
         <f t="shared" si="24"/>
-        <v>20.5</v>
+        <v>15.555555555555555</v>
       </c>
       <c r="Y43">
         <f t="shared" si="24"/>
-        <v>2.5</v>
+        <v>65</v>
       </c>
       <c r="Z43">
         <f t="shared" si="24"/>
-        <v>77</v>
+        <v>94.4</v>
       </c>
       <c r="AA43">
         <f t="shared" si="24"/>
-        <v>9.8000000000000007</v>
+        <v>23</v>
       </c>
       <c r="AB43" t="e">
         <f t="shared" si="24"/>
@@ -14188,7 +14802,7 @@
       </c>
       <c r="AC43">
         <f t="shared" si="24"/>
-        <v>2.6666666666666665</v>
+        <v>4</v>
       </c>
       <c r="AD43">
         <f t="shared" si="24"/>
@@ -14196,7 +14810,7 @@
       </c>
       <c r="AE43">
         <f t="shared" si="24"/>
-        <v>8</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="AF43">
         <f t="shared" si="24"/>
@@ -14208,7 +14822,7 @@
       </c>
       <c r="AH43">
         <f t="shared" si="24"/>
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="AI43" t="e">
         <f t="shared" si="24"/>
@@ -14216,11 +14830,11 @@
       </c>
       <c r="AJ43">
         <f t="shared" si="24"/>
-        <v>2.5</v>
+        <v>91.6</v>
       </c>
       <c r="AK43">
         <f t="shared" si="24"/>
-        <v>13</v>
+        <v>142.5</v>
       </c>
       <c r="AL43" t="e">
         <f t="shared" si="24"/>
@@ -14228,19 +14842,19 @@
       </c>
       <c r="AM43">
         <f t="shared" si="24"/>
-        <v>28</v>
-      </c>
-      <c r="AN43" t="e">
+        <v>14.111111111111111</v>
+      </c>
+      <c r="AN43">
         <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="AO43">
         <f t="shared" si="24"/>
-        <v>4.75</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="AP43">
         <f t="shared" si="24"/>
-        <v>122.75</v>
+        <v>59</v>
       </c>
       <c r="AQ43" t="e">
         <f t="shared" si="24"/>
@@ -14260,7 +14874,7 @@
       </c>
       <c r="AU43">
         <f t="shared" si="24"/>
-        <v>183.75</v>
+        <v>180.5</v>
       </c>
       <c r="AV43" t="e">
         <f t="shared" si="24"/>
@@ -14268,7 +14882,7 @@
       </c>
       <c r="AW43">
         <f t="shared" si="24"/>
-        <v>105.33333333333333</v>
+        <v>138</v>
       </c>
       <c r="AX43" t="e">
         <f t="shared" si="24"/>
@@ -14276,11 +14890,11 @@
       </c>
       <c r="AY43">
         <f t="shared" si="24"/>
-        <v>55</v>
+        <v>30.666666666666668</v>
       </c>
       <c r="AZ43">
         <f t="shared" si="24"/>
-        <v>124</v>
+        <v>262.83333333333331</v>
       </c>
     </row>
     <row r="44" spans="3:102">
@@ -14290,7 +14904,7 @@
       </c>
       <c r="D44">
         <f t="shared" ref="D44:AZ44" si="25">IF(ISNUMBER(D43),D43,"")</f>
-        <v>4.8</v>
+        <v>6.1111111111111107</v>
       </c>
       <c r="E44">
         <f t="shared" si="25"/>
@@ -14298,11 +14912,11 @@
       </c>
       <c r="F44">
         <f t="shared" si="25"/>
-        <v>1.75</v>
+        <v>3</v>
       </c>
       <c r="G44">
         <f t="shared" si="25"/>
-        <v>4</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="25"/>
@@ -14310,19 +14924,19 @@
       </c>
       <c r="I44">
         <f t="shared" si="25"/>
-        <v>3.2</v>
-      </c>
-      <c r="J44" t="str">
+        <v>3.4</v>
+      </c>
+      <c r="J44">
         <f t="shared" si="25"/>
-        <v/>
+        <v>4.5</v>
       </c>
       <c r="K44">
         <f t="shared" si="25"/>
-        <v>5.75</v>
+        <v>6.1428571428571432</v>
       </c>
       <c r="L44">
         <f t="shared" si="25"/>
-        <v>2.75</v>
+        <v>2.875</v>
       </c>
       <c r="M44" t="str">
         <f t="shared" si="25"/>
@@ -14330,19 +14944,19 @@
       </c>
       <c r="N44">
         <f t="shared" si="25"/>
-        <v>4.5999999999999996</v>
+        <v>5.9</v>
       </c>
       <c r="O44">
         <f t="shared" si="25"/>
-        <v>11</v>
+        <v>7.5</v>
       </c>
       <c r="P44">
         <f t="shared" si="25"/>
-        <v>7.666666666666667</v>
+        <v>6.833333333333333</v>
       </c>
       <c r="Q44">
         <f t="shared" si="25"/>
-        <v>3</v>
+        <v>3.5555555555555554</v>
       </c>
       <c r="R44" t="str">
         <f t="shared" si="25"/>
@@ -14350,7 +14964,7 @@
       </c>
       <c r="S44">
         <f t="shared" si="25"/>
-        <v>34.4</v>
+        <v>105.22222222222223</v>
       </c>
       <c r="T44" t="str">
         <f t="shared" si="25"/>
@@ -14358,11 +14972,11 @@
       </c>
       <c r="U44">
         <f t="shared" si="25"/>
-        <v>86</v>
+        <v>44.75</v>
       </c>
       <c r="V44">
         <f t="shared" si="25"/>
-        <v>3.3333333333333335</v>
+        <v>22.833333333333332</v>
       </c>
       <c r="W44" t="str">
         <f t="shared" si="25"/>
@@ -14370,19 +14984,19 @@
       </c>
       <c r="X44">
         <f t="shared" si="25"/>
-        <v>20.5</v>
+        <v>15.555555555555555</v>
       </c>
       <c r="Y44">
         <f t="shared" si="25"/>
-        <v>2.5</v>
+        <v>65</v>
       </c>
       <c r="Z44">
         <f t="shared" si="25"/>
-        <v>77</v>
+        <v>94.4</v>
       </c>
       <c r="AA44">
         <f t="shared" si="25"/>
-        <v>9.8000000000000007</v>
+        <v>23</v>
       </c>
       <c r="AB44" t="str">
         <f t="shared" si="25"/>
@@ -14390,7 +15004,7 @@
       </c>
       <c r="AC44">
         <f t="shared" si="25"/>
-        <v>2.6666666666666665</v>
+        <v>4</v>
       </c>
       <c r="AD44">
         <f t="shared" si="25"/>
@@ -14398,7 +15012,7 @@
       </c>
       <c r="AE44">
         <f t="shared" si="25"/>
-        <v>8</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="AF44">
         <f t="shared" si="25"/>
@@ -14410,7 +15024,7 @@
       </c>
       <c r="AH44">
         <f t="shared" si="25"/>
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="AI44" t="str">
         <f t="shared" si="25"/>
@@ -14418,11 +15032,11 @@
       </c>
       <c r="AJ44">
         <f t="shared" si="25"/>
-        <v>2.5</v>
+        <v>91.6</v>
       </c>
       <c r="AK44">
         <f t="shared" si="25"/>
-        <v>13</v>
+        <v>142.5</v>
       </c>
       <c r="AL44" t="str">
         <f t="shared" si="25"/>
@@ -14430,19 +15044,19 @@
       </c>
       <c r="AM44">
         <f t="shared" si="25"/>
-        <v>28</v>
-      </c>
-      <c r="AN44" t="str">
+        <v>14.111111111111111</v>
+      </c>
+      <c r="AN44">
         <f t="shared" si="25"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AO44">
         <f t="shared" si="25"/>
-        <v>4.75</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="AP44">
         <f t="shared" si="25"/>
-        <v>122.75</v>
+        <v>59</v>
       </c>
       <c r="AQ44" t="str">
         <f t="shared" si="25"/>
@@ -14462,7 +15076,7 @@
       </c>
       <c r="AU44">
         <f t="shared" si="25"/>
-        <v>183.75</v>
+        <v>180.5</v>
       </c>
       <c r="AV44" t="str">
         <f t="shared" si="25"/>
@@ -14470,7 +15084,7 @@
       </c>
       <c r="AW44">
         <f t="shared" si="25"/>
-        <v>105.33333333333333</v>
+        <v>138</v>
       </c>
       <c r="AX44" t="str">
         <f t="shared" si="25"/>
@@ -14478,11 +15092,11 @@
       </c>
       <c r="AY44">
         <f t="shared" si="25"/>
-        <v>55</v>
+        <v>30.666666666666668</v>
       </c>
       <c r="AZ44">
         <f t="shared" si="25"/>
-        <v>124</v>
+        <v>262.83333333333331</v>
       </c>
     </row>
     <row r="48" spans="3:102">
@@ -14496,11 +15110,11 @@
     <row r="49" spans="3:23">
       <c r="C49">
         <f>AVERAGE(C44:AA44)</f>
-        <v>16.725000000000001</v>
+        <v>23.43398078529658</v>
       </c>
       <c r="D49">
         <f>AVERAGE(AB44:AZ44)</f>
-        <v>71.75</v>
+        <v>87.409477124183013</v>
       </c>
     </row>
     <row r="51" spans="3:23">
@@ -14528,23 +15142,23 @@
     <row r="52" spans="3:23">
       <c r="C52">
         <f>AVERAGE(C44:G44,AB44:AF44)</f>
-        <v>5.6520833333333336</v>
+        <v>12.638888888888889</v>
       </c>
       <c r="H52">
         <f>AVERAGE(H44:L44,AG44:AK44)</f>
-        <v>4.9916666666666663</v>
+        <v>36.323979591836732</v>
       </c>
       <c r="M52">
         <f>AVERAGE(M44:Q44,AL44:AP44)</f>
-        <v>25.966666666666665</v>
+        <v>12.820833333333333</v>
       </c>
       <c r="R52">
         <f>AVERAGE(R44:V44,AQ44:AU44)</f>
-        <v>132.99722222222223</v>
+        <v>140.63425925925927</v>
       </c>
       <c r="W52">
         <f>AVERAGE(W44:AA44,AV44:AZ44)</f>
-        <v>56.304761904761904</v>
+        <v>89.922222222222217</v>
       </c>
     </row>
     <row r="55" spans="3:23">
@@ -14576,19 +15190,19 @@
       </c>
       <c r="D56">
         <f>AVERAGE(D44,I44,N44,S44,X44,AC44,AH44,AM44,AR44,AW44)</f>
-        <v>31.175000000000001</v>
+        <v>40.105000000000004</v>
       </c>
       <c r="E56">
         <f>AVERAGE(E44,J44,O44,T44,Y44,AD44,AI44,AN44,AS44,AX44)</f>
-        <v>8.375</v>
+        <v>16.333333333333332</v>
       </c>
       <c r="F56">
         <f>AVERAGE(F44,K44,P44,U44,Z44,AE44,AJ44,AO44,AT44,AY44)</f>
-        <v>63.341666666666676</v>
+        <v>72.539285714285725</v>
       </c>
       <c r="G56">
         <f>AVERAGE(G44,L44,Q44,V44,AA44,AF44,AK44,AP44,AU44,AZ44)</f>
-        <v>47.038333333333334</v>
+        <v>70.676388888888894</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pilot 1 - User 6.
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="target" sheetId="1" r:id="rId1"/>
     <sheet name="distance" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="117">
   <si>
     <t>userID</t>
   </si>
@@ -936,33 +937,33 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.4920000000000001</c:v>
+                  <c:v>0.4933333333333334</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.33199999999999996</c:v>
+                  <c:v>0.30333333333333334</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="49417216"/>
-        <c:axId val="49419008"/>
+        <c:axId val="50737920"/>
+        <c:axId val="50739456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="49417216"/>
+        <c:axId val="50737920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49419008"/>
+        <c:crossAx val="50739456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49419008"/>
+        <c:axId val="50739456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -972,7 +973,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49417216"/>
+        <c:crossAx val="50737920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -981,7 +982,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1029,42 +1030,42 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.4</c:v>
+                  <c:v>0.39166666666666672</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.44000000000000006</c:v>
+                  <c:v>0.44166666666666671</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.52</c:v>
+                  <c:v>0.5083333333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>0.26666666666666672</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.41999999999999993</c:v>
+                  <c:v>0.38333333333333336</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="49438080"/>
-        <c:axId val="49456256"/>
+        <c:axId val="50758784"/>
+        <c:axId val="50760320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="49438080"/>
+        <c:axId val="50758784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49456256"/>
+        <c:crossAx val="50760320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49456256"/>
+        <c:axId val="50760320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1074,7 +1075,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49438080"/>
+        <c:crossAx val="50758784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1083,7 +1084,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1131,42 +1132,42 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8.3333333333333332E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.81000000000000016</c:v>
+                  <c:v>0.74166666666666681</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1</c:v>
+                  <c:v>0.12499999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.45999999999999985</c:v>
+                  <c:v>0.47499999999999992</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.69000000000000006</c:v>
+                  <c:v>0.64166666666666661</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="50204672"/>
-        <c:axId val="50206208"/>
+        <c:axId val="51254784"/>
+        <c:axId val="51256320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50204672"/>
+        <c:axId val="51254784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50206208"/>
+        <c:crossAx val="51256320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50206208"/>
+        <c:axId val="51256320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1174,7 +1175,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50204672"/>
+        <c:crossAx val="51254784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1183,7 +1184,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1369,16 +1370,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1</c:v>
+                  <c:v>0.16666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.9</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1387,156 +1388,156 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.2</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.7</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.8</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.2</c:v>
+                  <c:v>0.16666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.6</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.9</c:v>
+                  <c:v>0.91666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.9</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.4</c:v>
+                  <c:v>0.41666666666666669</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.6</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.9</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.3</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.8</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.7</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.1</c:v>
+                  <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.3</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.4</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.8</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.4</c:v>
+                  <c:v>0.41666666666666669</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.9</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.1</c:v>
+                  <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.6</c:v>
+                  <c:v>0.58333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.9</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.2</c:v>
+                  <c:v>0.16666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.1</c:v>
+                  <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.6</c:v>
+                  <c:v>0.58333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.8</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.3</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.6</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="50229632"/>
-        <c:axId val="50231168"/>
+        <c:axId val="51296128"/>
+        <c:axId val="51297664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50229632"/>
+        <c:axId val="51296128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50231168"/>
+        <c:crossAx val="51297664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50231168"/>
+        <c:axId val="51297664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1546,7 +1547,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50229632"/>
+        <c:crossAx val="51296128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1555,7 +1556,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1603,24 +1604,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="50279168"/>
-        <c:axId val="50280704"/>
+        <c:axId val="51190016"/>
+        <c:axId val="51200000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50279168"/>
+        <c:axId val="51190016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50280704"/>
+        <c:crossAx val="51200000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50280704"/>
+        <c:axId val="51200000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1630,7 +1631,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50279168"/>
+        <c:crossAx val="51190016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1639,7 +1640,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1678,33 +1679,33 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>23.43398078529658</c:v>
+                  <c:v>22.925256132756132</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>87.409477124183013</c:v>
+                  <c:v>102.79098972922502</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="50828800"/>
-        <c:axId val="50830336"/>
+        <c:axId val="51338240"/>
+        <c:axId val="51340032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50828800"/>
+        <c:axId val="51338240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50830336"/>
+        <c:crossAx val="51340032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50830336"/>
+        <c:axId val="51340032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1712,7 +1713,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50828800"/>
+        <c:crossAx val="51338240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1721,7 +1722,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1769,42 +1770,42 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>12.638888888888889</c:v>
+                  <c:v>13.317857142857143</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.323979591836732</c:v>
+                  <c:v>36.664357864357861</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.820833333333333</c:v>
+                  <c:v>12.091053391053391</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>140.63425925925927</c:v>
+                  <c:v>159.7487528344671</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>89.922222222222217</c:v>
+                  <c:v>89.684126984126991</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="50337664"/>
-        <c:axId val="50339200"/>
+        <c:axId val="51355008"/>
+        <c:axId val="51364992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50337664"/>
+        <c:axId val="51355008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50339200"/>
+        <c:crossAx val="51364992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50339200"/>
+        <c:axId val="51364992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1812,7 +1813,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50337664"/>
+        <c:crossAx val="51355008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1821,7 +1822,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1872,39 +1873,39 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40.105000000000004</c:v>
+                  <c:v>40.294797979797977</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.333333333333332</c:v>
+                  <c:v>14.928571428571429</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>72.539285714285725</c:v>
+                  <c:v>73.117380952380955</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70.676388888888894</c:v>
+                  <c:v>96.733015873015873</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="50349952"/>
-        <c:axId val="50351488"/>
+        <c:axId val="50355584"/>
+        <c:axId val="51471488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50349952"/>
+        <c:axId val="50355584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50351488"/>
+        <c:crossAx val="51471488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50351488"/>
+        <c:axId val="51471488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1912,7 +1913,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50349952"/>
+        <c:crossAx val="50355584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1921,7 +1922,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2086,16 +2087,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>61</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1879890</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>19916</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>69</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1472047</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>96116</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2462,10 +2463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DA30"/>
+  <dimension ref="A1:DA55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="CS36" sqref="CS36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AI56" sqref="AI56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2485,7 +2486,9 @@
     <col min="18" max="18" width="27.140625" customWidth="1"/>
     <col min="19" max="22" width="12.7109375" customWidth="1"/>
     <col min="23" max="23" width="24.5703125" customWidth="1"/>
-    <col min="24" max="52" width="12.7109375" customWidth="1"/>
+    <col min="24" max="43" width="12.7109375" customWidth="1"/>
+    <col min="44" max="44" width="13.5703125" customWidth="1"/>
+    <col min="45" max="52" width="12.7109375" customWidth="1"/>
     <col min="53" max="53" width="28" customWidth="1"/>
     <col min="54" max="102" width="12.7109375" customWidth="1"/>
   </cols>
@@ -5006,7 +5009,7 @@
         <v>1</v>
       </c>
       <c r="DA7" s="1">
-        <f t="shared" ref="DA7:DA10" si="13">SUM(C7:CX7)</f>
+        <f t="shared" ref="DA7:DA11" si="13">SUM(C7:CX7)</f>
         <v>52</v>
       </c>
     </row>
@@ -5937,6 +5940,315 @@
         <v>36</v>
       </c>
     </row>
+    <row r="11" spans="1:105">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <v>1</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>1</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11">
+        <v>0</v>
+      </c>
+      <c r="AI11">
+        <v>0</v>
+      </c>
+      <c r="AJ11">
+        <v>0</v>
+      </c>
+      <c r="AK11">
+        <v>0</v>
+      </c>
+      <c r="AL11">
+        <v>0</v>
+      </c>
+      <c r="AM11">
+        <v>0</v>
+      </c>
+      <c r="AN11">
+        <v>0</v>
+      </c>
+      <c r="AO11">
+        <v>0</v>
+      </c>
+      <c r="AP11">
+        <v>1</v>
+      </c>
+      <c r="AQ11">
+        <v>0</v>
+      </c>
+      <c r="AR11">
+        <v>0</v>
+      </c>
+      <c r="AS11">
+        <v>0</v>
+      </c>
+      <c r="AT11">
+        <v>0</v>
+      </c>
+      <c r="AU11">
+        <v>1</v>
+      </c>
+      <c r="AV11">
+        <v>0</v>
+      </c>
+      <c r="AW11">
+        <v>0</v>
+      </c>
+      <c r="AX11">
+        <v>0</v>
+      </c>
+      <c r="AY11">
+        <v>0</v>
+      </c>
+      <c r="AZ11">
+        <v>0</v>
+      </c>
+      <c r="BA11">
+        <v>0</v>
+      </c>
+      <c r="BB11">
+        <v>0</v>
+      </c>
+      <c r="BC11">
+        <v>1</v>
+      </c>
+      <c r="BD11">
+        <v>1</v>
+      </c>
+      <c r="BE11">
+        <v>1</v>
+      </c>
+      <c r="BF11">
+        <v>0</v>
+      </c>
+      <c r="BG11">
+        <v>1</v>
+      </c>
+      <c r="BH11">
+        <v>0</v>
+      </c>
+      <c r="BI11">
+        <v>1</v>
+      </c>
+      <c r="BJ11">
+        <v>0</v>
+      </c>
+      <c r="BK11">
+        <v>1</v>
+      </c>
+      <c r="BL11">
+        <v>1</v>
+      </c>
+      <c r="BM11">
+        <v>0</v>
+      </c>
+      <c r="BN11">
+        <v>1</v>
+      </c>
+      <c r="BO11">
+        <v>1</v>
+      </c>
+      <c r="BP11">
+        <v>0</v>
+      </c>
+      <c r="BQ11">
+        <v>1</v>
+      </c>
+      <c r="BR11">
+        <v>0</v>
+      </c>
+      <c r="BS11">
+        <v>0</v>
+      </c>
+      <c r="BT11">
+        <v>0</v>
+      </c>
+      <c r="BU11">
+        <v>0</v>
+      </c>
+      <c r="BV11">
+        <v>1</v>
+      </c>
+      <c r="BW11">
+        <v>1</v>
+      </c>
+      <c r="BX11">
+        <v>1</v>
+      </c>
+      <c r="BY11">
+        <v>0</v>
+      </c>
+      <c r="BZ11">
+        <v>0</v>
+      </c>
+      <c r="CA11">
+        <v>1</v>
+      </c>
+      <c r="CB11">
+        <v>0</v>
+      </c>
+      <c r="CC11">
+        <v>1</v>
+      </c>
+      <c r="CD11">
+        <v>0</v>
+      </c>
+      <c r="CE11">
+        <v>0</v>
+      </c>
+      <c r="CF11">
+        <v>0</v>
+      </c>
+      <c r="CG11">
+        <v>1</v>
+      </c>
+      <c r="CH11">
+        <v>1</v>
+      </c>
+      <c r="CI11">
+        <v>1</v>
+      </c>
+      <c r="CJ11">
+        <v>0</v>
+      </c>
+      <c r="CK11">
+        <v>0</v>
+      </c>
+      <c r="CL11">
+        <v>0</v>
+      </c>
+      <c r="CM11">
+        <v>1</v>
+      </c>
+      <c r="CN11">
+        <v>0</v>
+      </c>
+      <c r="CO11">
+        <v>0</v>
+      </c>
+      <c r="CP11">
+        <v>0</v>
+      </c>
+      <c r="CQ11">
+        <v>0</v>
+      </c>
+      <c r="CR11">
+        <v>0</v>
+      </c>
+      <c r="CS11">
+        <v>0</v>
+      </c>
+      <c r="CT11">
+        <v>0</v>
+      </c>
+      <c r="CU11">
+        <v>0</v>
+      </c>
+      <c r="CV11">
+        <v>0</v>
+      </c>
+      <c r="CW11">
+        <v>0</v>
+      </c>
+      <c r="CX11">
+        <v>0</v>
+      </c>
+      <c r="DA11" s="1">
+        <f t="shared" si="13"/>
+        <v>33</v>
+      </c>
+    </row>
     <row r="16" spans="1:105">
       <c r="C16" t="s">
         <v>31</v>
@@ -5949,19 +6261,19 @@
       </c>
       <c r="D17">
         <f t="shared" ref="D17:AZ17" si="14">AVERAGE(D6:D14,BB6:BB15)</f>
-        <v>0.9</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E17">
         <f t="shared" si="14"/>
-        <v>0.1</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F17">
         <f t="shared" si="14"/>
-        <v>0.6</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G17">
         <f t="shared" si="14"/>
-        <v>0.9</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="H17">
         <f t="shared" si="14"/>
@@ -5973,19 +6285,19 @@
       </c>
       <c r="J17">
         <f t="shared" si="14"/>
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="K17">
         <f t="shared" si="14"/>
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="L17">
         <f t="shared" si="14"/>
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="M17">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="N17">
         <f t="shared" si="14"/>
@@ -5993,15 +6305,15 @@
       </c>
       <c r="O17">
         <f t="shared" si="14"/>
-        <v>0.2</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="P17">
         <f t="shared" si="14"/>
-        <v>0.6</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="Q17">
         <f t="shared" si="14"/>
-        <v>0.9</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="R17">
         <f t="shared" si="14"/>
@@ -6009,19 +6321,19 @@
       </c>
       <c r="S17">
         <f t="shared" si="14"/>
-        <v>0.9</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="T17">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="U17">
         <f t="shared" si="14"/>
-        <v>0.4</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="V17">
         <f t="shared" si="14"/>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="W17">
         <f t="shared" si="14"/>
@@ -6029,11 +6341,11 @@
       </c>
       <c r="X17">
         <f t="shared" si="14"/>
-        <v>0.9</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="Y17">
         <f t="shared" si="14"/>
-        <v>0.3</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="Z17">
         <f t="shared" si="14"/>
@@ -6041,7 +6353,7 @@
       </c>
       <c r="AA17">
         <f t="shared" si="14"/>
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="AB17">
         <f t="shared" si="14"/>
@@ -6049,19 +6361,19 @@
       </c>
       <c r="AC17">
         <f t="shared" si="14"/>
-        <v>0.7</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="AD17">
         <f t="shared" si="14"/>
-        <v>0.1</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="AE17">
         <f t="shared" si="14"/>
-        <v>0.3</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="AF17">
         <f t="shared" si="14"/>
-        <v>0.4</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="AG17">
         <f t="shared" si="14"/>
@@ -6069,11 +6381,11 @@
       </c>
       <c r="AH17">
         <f t="shared" si="14"/>
-        <v>0.8</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="AI17">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="AJ17">
         <f t="shared" si="14"/>
@@ -6081,7 +6393,7 @@
       </c>
       <c r="AK17">
         <f t="shared" si="14"/>
-        <v>0.4</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="AL17">
         <f t="shared" si="14"/>
@@ -6089,19 +6401,19 @@
       </c>
       <c r="AM17">
         <f t="shared" si="14"/>
-        <v>0.9</v>
+        <v>0.75</v>
       </c>
       <c r="AN17">
         <f t="shared" si="14"/>
-        <v>0.1</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="AO17">
         <f t="shared" si="14"/>
-        <v>0.6</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="AP17">
         <f t="shared" si="14"/>
-        <v>0.9</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="AQ17">
         <f t="shared" si="14"/>
@@ -6109,7 +6421,7 @@
       </c>
       <c r="AR17">
         <f t="shared" si="14"/>
-        <v>0.2</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="AS17">
         <f t="shared" si="14"/>
@@ -6117,11 +6429,11 @@
       </c>
       <c r="AT17">
         <f t="shared" si="14"/>
-        <v>0.1</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="AU17">
         <f t="shared" si="14"/>
-        <v>0.6</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="AV17">
         <f t="shared" si="14"/>
@@ -6129,7 +6441,7 @@
       </c>
       <c r="AW17">
         <f t="shared" si="14"/>
-        <v>0.8</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="AX17">
         <f t="shared" si="14"/>
@@ -6137,11 +6449,11 @@
       </c>
       <c r="AY17">
         <f t="shared" si="14"/>
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="AZ17">
         <f t="shared" si="14"/>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="3:52">
@@ -6155,11 +6467,11 @@
     <row r="20" spans="3:52">
       <c r="C20">
         <f>AVERAGE(C17:AA17)</f>
-        <v>0.4920000000000001</v>
+        <v>0.4933333333333334</v>
       </c>
       <c r="D20">
         <f>AVERAGE(AB17:AZ17)</f>
-        <v>0.33199999999999996</v>
+        <v>0.30333333333333334</v>
       </c>
     </row>
     <row r="22" spans="3:52">
@@ -6187,23 +6499,23 @@
     <row r="23" spans="3:52">
       <c r="C23">
         <f>AVERAGE(C17:G17,AB17:AF17)</f>
-        <v>0.4</v>
+        <v>0.39166666666666672</v>
       </c>
       <c r="H23">
         <f>AVERAGE(H17:L17,AG17:AK17)</f>
-        <v>0.44000000000000006</v>
+        <v>0.44166666666666671</v>
       </c>
       <c r="M23">
         <f>AVERAGE(M17:Q17,AL17:AP17)</f>
-        <v>0.52</v>
+        <v>0.5083333333333333</v>
       </c>
       <c r="R23">
         <f>AVERAGE(R17:V17,AQ17:AU17)</f>
-        <v>0.28000000000000003</v>
+        <v>0.26666666666666672</v>
       </c>
       <c r="W23">
         <f>AVERAGE(W17:AA17,AV17:AZ17)</f>
-        <v>0.41999999999999993</v>
+        <v>0.38333333333333336</v>
       </c>
     </row>
     <row r="25" spans="3:52">
@@ -6231,23 +6543,23 @@
     <row r="26" spans="3:52">
       <c r="C26">
         <f>AVERAGE(C17,H17,M17,R17,W17,AB17,AG17,AL17,AQ17,AV17)</f>
-        <v>0</v>
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="D26">
         <f t="shared" ref="D26:G26" si="16">AVERAGE(D17,I17,N17,S17,X17,AC17,AH17,AM17,AR17,AW17)</f>
-        <v>0.81000000000000016</v>
+        <v>0.74166666666666681</v>
       </c>
       <c r="E26">
         <f t="shared" si="16"/>
-        <v>0.1</v>
+        <v>0.12499999999999997</v>
       </c>
       <c r="F26">
         <f t="shared" si="16"/>
-        <v>0.45999999999999985</v>
+        <v>0.47499999999999992</v>
       </c>
       <c r="G26">
         <f t="shared" si="16"/>
-        <v>0.69000000000000006</v>
+        <v>0.64166666666666661</v>
       </c>
     </row>
     <row r="29" spans="3:52">
@@ -6270,7 +6582,362 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="34" spans="2:7">
+      <c r="C34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7">
+      <c r="C35" t="str">
+        <f>C25</f>
+        <v>Amplitude 0</v>
+      </c>
+      <c r="D35" t="str">
+        <f>E25</f>
+        <v>Amplitude 25</v>
+      </c>
+      <c r="E35" t="str">
+        <f>F25</f>
+        <v>Amplitude 50</v>
+      </c>
+      <c r="F35" t="str">
+        <f>G25</f>
+        <v>Amplitude 75</v>
+      </c>
+      <c r="G35" t="str">
+        <f>D25</f>
+        <v>Amplitude 100</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36" t="str">
+        <f>R22</f>
+        <v>Duration 250</v>
+      </c>
+      <c r="C36">
+        <f>R17</f>
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <f>T17</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E36">
+        <f>U17</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F36">
+        <f>V17</f>
+        <v>0.5</v>
+      </c>
+      <c r="G36">
+        <f>S17</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" t="str">
+        <f>W22</f>
+        <v>Duration 500</v>
+      </c>
+      <c r="C37">
+        <f>W17</f>
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <f>Y17</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E37">
+        <f>Z17</f>
+        <v>0.5</v>
+      </c>
+      <c r="F37">
+        <f>AA17</f>
+        <v>0.75</v>
+      </c>
+      <c r="G37">
+        <f>X17</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" t="str">
+        <f>C22</f>
+        <v>Duration 1000</v>
+      </c>
+      <c r="C38">
+        <f>C17</f>
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <f>E17</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E38">
+        <f>F17</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F38">
+        <f>G17</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G38">
+        <f>D17</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39" t="str">
+        <f>H22</f>
+        <v>Duration 1500</v>
+      </c>
+      <c r="C39">
+        <f>H17</f>
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <f>J17</f>
+        <v>0.25</v>
+      </c>
+      <c r="E39">
+        <f>K17</f>
+        <v>0.75</v>
+      </c>
+      <c r="F39">
+        <f>L17</f>
+        <v>0.75</v>
+      </c>
+      <c r="G39">
+        <f>I17</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7">
+      <c r="B40" t="str">
+        <f>M22</f>
+        <v>Duration 2000</v>
+      </c>
+      <c r="C40">
+        <f>M17</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D40">
+        <f>O17</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E40">
+        <f>P17</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F40">
+        <f>Q17</f>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="G40">
+        <f>N17</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7">
+      <c r="C46" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7">
+      <c r="C47" t="str">
+        <f>C35</f>
+        <v>Amplitude 0</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" ref="D47:G47" si="17">D35</f>
+        <v>Amplitude 25</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="17"/>
+        <v>Amplitude 50</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="17"/>
+        <v>Amplitude 75</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="17"/>
+        <v>Amplitude 100</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7">
+      <c r="B48" t="str">
+        <f>B36</f>
+        <v>Duration 250</v>
+      </c>
+      <c r="C48">
+        <f>AQ17</f>
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <f>AS17</f>
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <f>AT17</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F48">
+        <f>AU17</f>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G48">
+        <f>AR17</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7">
+      <c r="B49" t="str">
+        <f t="shared" ref="B49:B52" si="18">B37</f>
+        <v>Duration 500</v>
+      </c>
+      <c r="C49">
+        <f>W17</f>
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <f>AX17</f>
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <f>AY17</f>
+        <v>0.25</v>
+      </c>
+      <c r="F49">
+        <f>AZ17</f>
+        <v>0.5</v>
+      </c>
+      <c r="G49">
+        <f>AW17</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7">
+      <c r="B50" t="str">
+        <f t="shared" si="18"/>
+        <v>Duration 1000</v>
+      </c>
+      <c r="C50">
+        <f>AB17</f>
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <f>AD17</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E50">
+        <f>AE17</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F50">
+        <f>AF17</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G50">
+        <f>AC17</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7">
+      <c r="B51" t="str">
+        <f t="shared" si="18"/>
+        <v>Duration 1500</v>
+      </c>
+      <c r="C51">
+        <f>AG17</f>
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <f>AI17</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E51">
+        <f>AJ17</f>
+        <v>0.5</v>
+      </c>
+      <c r="F51">
+        <f>AK17</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G51">
+        <f>AH17</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7">
+      <c r="B52" t="str">
+        <f t="shared" si="18"/>
+        <v>Duration 2000</v>
+      </c>
+      <c r="C52">
+        <f>AL17</f>
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <f>AN17</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E52">
+        <f>AO17</f>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F52">
+        <f>AP17</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G52">
+        <f>AM17</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7">
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0.25</v>
+      </c>
+      <c r="E55">
+        <v>0.5</v>
+      </c>
+      <c r="F55">
+        <v>0.75</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="C36:G40">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48:G52 C55:G55">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -6279,16 +6946,73 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CX56"/>
+  <dimension ref="A1:CX79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M86" sqref="M86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="52" max="52" width="21.28515625" customWidth="1"/>
-    <col min="53" max="53" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="28" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="37" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="42" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="47" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="53" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="57" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="62" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="65" max="67" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="70" max="72" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="75" max="78" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="80" max="82" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="85" max="87" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="90" max="92" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="95" max="97" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="100" max="102" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:102">
@@ -9866,6 +10590,311 @@
         <v>150</v>
       </c>
     </row>
+    <row r="11" spans="1:102">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>-1</v>
+      </c>
+      <c r="D11">
+        <v>19</v>
+      </c>
+      <c r="E11">
+        <v>-1</v>
+      </c>
+      <c r="F11">
+        <v>32</v>
+      </c>
+      <c r="G11">
+        <v>-1</v>
+      </c>
+      <c r="H11">
+        <v>-1</v>
+      </c>
+      <c r="I11">
+        <v>13</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>7</v>
+      </c>
+      <c r="L11">
+        <v>11</v>
+      </c>
+      <c r="M11">
+        <v>-1</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="O11">
+        <v>-1</v>
+      </c>
+      <c r="P11">
+        <v>6</v>
+      </c>
+      <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="R11">
+        <v>-1</v>
+      </c>
+      <c r="S11">
+        <v>-1</v>
+      </c>
+      <c r="T11">
+        <v>6</v>
+      </c>
+      <c r="U11">
+        <v>53</v>
+      </c>
+      <c r="V11">
+        <v>-1</v>
+      </c>
+      <c r="W11">
+        <v>-1</v>
+      </c>
+      <c r="X11">
+        <v>-1</v>
+      </c>
+      <c r="Y11">
+        <v>-1</v>
+      </c>
+      <c r="Z11">
+        <v>-1</v>
+      </c>
+      <c r="AA11">
+        <v>8</v>
+      </c>
+      <c r="AB11">
+        <v>-1</v>
+      </c>
+      <c r="AC11">
+        <v>-1</v>
+      </c>
+      <c r="AD11">
+        <v>-1</v>
+      </c>
+      <c r="AE11">
+        <v>-1</v>
+      </c>
+      <c r="AF11">
+        <v>-1</v>
+      </c>
+      <c r="AG11">
+        <v>-1</v>
+      </c>
+      <c r="AH11">
+        <v>-1</v>
+      </c>
+      <c r="AI11">
+        <v>-1</v>
+      </c>
+      <c r="AJ11">
+        <v>-1</v>
+      </c>
+      <c r="AK11">
+        <v>-1</v>
+      </c>
+      <c r="AL11">
+        <v>-1</v>
+      </c>
+      <c r="AM11">
+        <v>-1</v>
+      </c>
+      <c r="AN11">
+        <v>-1</v>
+      </c>
+      <c r="AO11">
+        <v>-1</v>
+      </c>
+      <c r="AP11">
+        <v>6</v>
+      </c>
+      <c r="AQ11">
+        <v>-1</v>
+      </c>
+      <c r="AR11">
+        <v>-1</v>
+      </c>
+      <c r="AS11">
+        <v>-1</v>
+      </c>
+      <c r="AT11">
+        <v>-1</v>
+      </c>
+      <c r="AU11">
+        <v>2048</v>
+      </c>
+      <c r="AV11">
+        <v>-1</v>
+      </c>
+      <c r="AW11">
+        <v>-1</v>
+      </c>
+      <c r="AX11">
+        <v>-1</v>
+      </c>
+      <c r="AY11">
+        <v>-1</v>
+      </c>
+      <c r="AZ11">
+        <v>-1</v>
+      </c>
+      <c r="BA11">
+        <v>-1</v>
+      </c>
+      <c r="BB11">
+        <v>-1</v>
+      </c>
+      <c r="BC11">
+        <v>4</v>
+      </c>
+      <c r="BD11">
+        <v>286</v>
+      </c>
+      <c r="BE11">
+        <v>8</v>
+      </c>
+      <c r="BF11">
+        <v>-1</v>
+      </c>
+      <c r="BG11">
+        <v>3</v>
+      </c>
+      <c r="BH11">
+        <v>-1</v>
+      </c>
+      <c r="BI11">
+        <v>9</v>
+      </c>
+      <c r="BJ11">
+        <v>-1</v>
+      </c>
+      <c r="BK11">
+        <v>726</v>
+      </c>
+      <c r="BL11">
+        <v>6</v>
+      </c>
+      <c r="BM11">
+        <v>-1</v>
+      </c>
+      <c r="BN11">
+        <v>5</v>
+      </c>
+      <c r="BO11">
+        <v>13</v>
+      </c>
+      <c r="BP11">
+        <v>-1</v>
+      </c>
+      <c r="BQ11">
+        <v>131</v>
+      </c>
+      <c r="BR11">
+        <v>-1</v>
+      </c>
+      <c r="BS11">
+        <v>-1</v>
+      </c>
+      <c r="BT11">
+        <v>-1</v>
+      </c>
+      <c r="BU11">
+        <v>-1</v>
+      </c>
+      <c r="BV11">
+        <v>5</v>
+      </c>
+      <c r="BW11">
+        <v>306</v>
+      </c>
+      <c r="BX11">
+        <v>38</v>
+      </c>
+      <c r="BY11">
+        <v>-1</v>
+      </c>
+      <c r="BZ11">
+        <v>-1</v>
+      </c>
+      <c r="CA11">
+        <v>8</v>
+      </c>
+      <c r="CB11">
+        <v>-1</v>
+      </c>
+      <c r="CC11">
+        <v>1799</v>
+      </c>
+      <c r="CD11">
+        <v>-1</v>
+      </c>
+      <c r="CE11">
+        <v>-1</v>
+      </c>
+      <c r="CF11">
+        <v>-1</v>
+      </c>
+      <c r="CG11">
+        <v>34</v>
+      </c>
+      <c r="CH11">
+        <v>3185</v>
+      </c>
+      <c r="CI11">
+        <v>110</v>
+      </c>
+      <c r="CJ11">
+        <v>-1</v>
+      </c>
+      <c r="CK11">
+        <v>-1</v>
+      </c>
+      <c r="CL11">
+        <v>-1</v>
+      </c>
+      <c r="CM11">
+        <v>8</v>
+      </c>
+      <c r="CN11">
+        <v>-1</v>
+      </c>
+      <c r="CO11">
+        <v>-1</v>
+      </c>
+      <c r="CP11">
+        <v>-1</v>
+      </c>
+      <c r="CQ11">
+        <v>-1</v>
+      </c>
+      <c r="CR11">
+        <v>-1</v>
+      </c>
+      <c r="CS11">
+        <v>-1</v>
+      </c>
+      <c r="CT11">
+        <v>-1</v>
+      </c>
+      <c r="CU11">
+        <v>-1</v>
+      </c>
+      <c r="CV11">
+        <v>-1</v>
+      </c>
+      <c r="CW11">
+        <v>-1</v>
+      </c>
+      <c r="CX11">
+        <v>-1</v>
+      </c>
+    </row>
     <row r="22" spans="3:102">
       <c r="C22" t="str">
         <f>IF(C6&gt;=0,C6,"")</f>
@@ -11877,405 +12906,405 @@
       </c>
     </row>
     <row r="27" spans="3:102">
-      <c r="C27">
+      <c r="C27" t="str">
         <f t="shared" ref="C27:BN27" si="10">IF(C11&gt;=0,C11,"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D27">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="E27">
+        <v>19</v>
+      </c>
+      <c r="E27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="F27">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="G27">
+        <v>32</v>
+      </c>
+      <c r="G27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="H27">
+        <v/>
+      </c>
+      <c r="H27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="I27">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J27">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K27">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L27">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="M27">
+        <v>11</v>
+      </c>
+      <c r="M27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="N27">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="O27">
+        <v>3</v>
+      </c>
+      <c r="O27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="P27">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q27">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="R27">
+        <v>2</v>
+      </c>
+      <c r="R27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="S27">
+        <v/>
+      </c>
+      <c r="S27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="T27">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U27">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="V27">
+        <v>53</v>
+      </c>
+      <c r="V27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="W27">
+        <v/>
+      </c>
+      <c r="W27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="X27">
+        <v/>
+      </c>
+      <c r="X27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Y27">
+        <v/>
+      </c>
+      <c r="Y27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Z27">
+        <v/>
+      </c>
+      <c r="Z27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AA27">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB27">
+        <v>8</v>
+      </c>
+      <c r="AB27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AC27">
+        <v/>
+      </c>
+      <c r="AC27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AD27">
+        <v/>
+      </c>
+      <c r="AD27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AE27">
+        <v/>
+      </c>
+      <c r="AE27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AF27">
+        <v/>
+      </c>
+      <c r="AF27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AG27">
+        <v/>
+      </c>
+      <c r="AG27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AH27">
+        <v/>
+      </c>
+      <c r="AH27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AI27">
+        <v/>
+      </c>
+      <c r="AI27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AJ27">
+        <v/>
+      </c>
+      <c r="AJ27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AK27">
+        <v/>
+      </c>
+      <c r="AK27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AL27">
+        <v/>
+      </c>
+      <c r="AL27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AM27">
+        <v/>
+      </c>
+      <c r="AM27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AN27">
+        <v/>
+      </c>
+      <c r="AN27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AO27">
+        <v/>
+      </c>
+      <c r="AO27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AP27">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AQ27">
+        <v>6</v>
+      </c>
+      <c r="AQ27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AR27">
+        <v/>
+      </c>
+      <c r="AR27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AS27">
+        <v/>
+      </c>
+      <c r="AS27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AT27">
+        <v/>
+      </c>
+      <c r="AT27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AU27">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AV27">
+        <v>2048</v>
+      </c>
+      <c r="AV27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AW27">
+        <v/>
+      </c>
+      <c r="AW27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AX27">
+        <v/>
+      </c>
+      <c r="AX27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AY27">
+        <v/>
+      </c>
+      <c r="AY27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AZ27">
+        <v/>
+      </c>
+      <c r="AZ27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="BA27">
+        <v/>
+      </c>
+      <c r="BA27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="BB27">
+        <v/>
+      </c>
+      <c r="BB27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BC27">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BD27">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>286</v>
       </c>
       <c r="BE27">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="BF27">
+        <v>8</v>
+      </c>
+      <c r="BF27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BG27">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="BH27">
+        <v>3</v>
+      </c>
+      <c r="BH27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BI27">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="BJ27">
+        <v>9</v>
+      </c>
+      <c r="BJ27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BK27">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>726</v>
       </c>
       <c r="BL27">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="BM27">
+        <v>6</v>
+      </c>
+      <c r="BM27" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BN27">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BO27">
         <f t="shared" ref="BO27:CX27" si="11">IF(BO11&gt;=0,BO11,"")</f>
-        <v>0</v>
-      </c>
-      <c r="BP27">
+        <v>13</v>
+      </c>
+      <c r="BP27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BQ27">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="BR27">
+        <v>131</v>
+      </c>
+      <c r="BR27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="BS27">
+        <v/>
+      </c>
+      <c r="BS27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="BT27">
+        <v/>
+      </c>
+      <c r="BT27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="BU27">
+        <v/>
+      </c>
+      <c r="BU27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BV27">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BW27">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>306</v>
       </c>
       <c r="BX27">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="BY27">
+        <v>38</v>
+      </c>
+      <c r="BY27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="BZ27">
+        <v/>
+      </c>
+      <c r="BZ27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CA27">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="CB27">
+        <v>8</v>
+      </c>
+      <c r="CB27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CC27">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="CD27">
+        <v>1799</v>
+      </c>
+      <c r="CD27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="CE27">
+        <v/>
+      </c>
+      <c r="CE27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="CF27">
+        <v/>
+      </c>
+      <c r="CF27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CG27">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="CH27">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>3185</v>
       </c>
       <c r="CI27">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="CJ27">
+        <v>110</v>
+      </c>
+      <c r="CJ27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="CK27">
+        <v/>
+      </c>
+      <c r="CK27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="CL27">
+        <v/>
+      </c>
+      <c r="CL27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="CM27">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="CN27">
+        <v>8</v>
+      </c>
+      <c r="CN27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="CO27">
+        <v/>
+      </c>
+      <c r="CO27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="CP27">
+        <v/>
+      </c>
+      <c r="CP27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="CQ27">
+        <v/>
+      </c>
+      <c r="CQ27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="CR27">
+        <v/>
+      </c>
+      <c r="CR27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="CS27">
+        <v/>
+      </c>
+      <c r="CS27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="CT27">
+        <v/>
+      </c>
+      <c r="CT27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="CU27">
+        <v/>
+      </c>
+      <c r="CU27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="CV27">
+        <v/>
+      </c>
+      <c r="CV27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="CW27">
+        <v/>
+      </c>
+      <c r="CW27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="CX27">
+        <v/>
+      </c>
+      <c r="CX27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="28" spans="3:102">
@@ -14697,12 +15726,12 @@
     </row>
     <row r="43" spans="3:102">
       <c r="C43" t="e">
-        <f>AVERAGE(C22:C26,BA22:BA26)</f>
+        <f>AVERAGE(C22:C27,BA22:BA26)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D43">
-        <f t="shared" ref="D43:AZ43" si="24">AVERAGE(D22:D26,BB22:BB26)</f>
-        <v>6.1111111111111107</v>
+        <f t="shared" ref="D43:AZ43" si="24">AVERAGE(D22:D27,BB22:BB26)</f>
+        <v>7.4</v>
       </c>
       <c r="E43">
         <f t="shared" si="24"/>
@@ -14710,7 +15739,7 @@
       </c>
       <c r="F43">
         <f t="shared" si="24"/>
-        <v>3</v>
+        <v>7.1428571428571432</v>
       </c>
       <c r="G43">
         <f t="shared" si="24"/>
@@ -14722,19 +15751,19 @@
       </c>
       <c r="I43">
         <f t="shared" si="24"/>
-        <v>3.4</v>
+        <v>4.2727272727272725</v>
       </c>
       <c r="J43">
         <f t="shared" si="24"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="K43">
         <f t="shared" si="24"/>
-        <v>6.1428571428571432</v>
+        <v>6.25</v>
       </c>
       <c r="L43">
         <f t="shared" si="24"/>
-        <v>2.875</v>
+        <v>3.7777777777777777</v>
       </c>
       <c r="M43" t="e">
         <f t="shared" si="24"/>
@@ -14742,7 +15771,7 @@
       </c>
       <c r="N43">
         <f t="shared" si="24"/>
-        <v>5.9</v>
+        <v>5.6363636363636367</v>
       </c>
       <c r="O43">
         <f t="shared" si="24"/>
@@ -14750,11 +15779,11 @@
       </c>
       <c r="P43">
         <f t="shared" si="24"/>
-        <v>6.833333333333333</v>
+        <v>6.7142857142857144</v>
       </c>
       <c r="Q43">
         <f t="shared" si="24"/>
-        <v>3.5555555555555554</v>
+        <v>3.4</v>
       </c>
       <c r="R43" t="e">
         <f t="shared" si="24"/>
@@ -14764,13 +15793,13 @@
         <f t="shared" si="24"/>
         <v>105.22222222222223</v>
       </c>
-      <c r="T43" t="e">
+      <c r="T43">
         <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
+        <v>6</v>
       </c>
       <c r="U43">
         <f t="shared" si="24"/>
-        <v>44.75</v>
+        <v>46.4</v>
       </c>
       <c r="V43">
         <f t="shared" si="24"/>
@@ -14794,7 +15823,7 @@
       </c>
       <c r="AA43">
         <f t="shared" si="24"/>
-        <v>23</v>
+        <v>21.333333333333332</v>
       </c>
       <c r="AB43" t="e">
         <f t="shared" si="24"/>
@@ -14854,7 +15883,7 @@
       </c>
       <c r="AP43">
         <f t="shared" si="24"/>
-        <v>59</v>
+        <v>53.7</v>
       </c>
       <c r="AQ43" t="e">
         <f t="shared" si="24"/>
@@ -14874,7 +15903,7 @@
       </c>
       <c r="AU43">
         <f t="shared" si="24"/>
-        <v>180.5</v>
+        <v>447.28571428571428</v>
       </c>
       <c r="AV43" t="e">
         <f t="shared" si="24"/>
@@ -14904,7 +15933,7 @@
       </c>
       <c r="D44">
         <f t="shared" ref="D44:AZ44" si="25">IF(ISNUMBER(D43),D43,"")</f>
-        <v>6.1111111111111107</v>
+        <v>7.4</v>
       </c>
       <c r="E44">
         <f t="shared" si="25"/>
@@ -14912,7 +15941,7 @@
       </c>
       <c r="F44">
         <f t="shared" si="25"/>
-        <v>3</v>
+        <v>7.1428571428571432</v>
       </c>
       <c r="G44">
         <f t="shared" si="25"/>
@@ -14924,19 +15953,19 @@
       </c>
       <c r="I44">
         <f t="shared" si="25"/>
-        <v>3.4</v>
+        <v>4.2727272727272725</v>
       </c>
       <c r="J44">
         <f t="shared" si="25"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="K44">
         <f t="shared" si="25"/>
-        <v>6.1428571428571432</v>
+        <v>6.25</v>
       </c>
       <c r="L44">
         <f t="shared" si="25"/>
-        <v>2.875</v>
+        <v>3.7777777777777777</v>
       </c>
       <c r="M44" t="str">
         <f t="shared" si="25"/>
@@ -14944,7 +15973,7 @@
       </c>
       <c r="N44">
         <f t="shared" si="25"/>
-        <v>5.9</v>
+        <v>5.6363636363636367</v>
       </c>
       <c r="O44">
         <f t="shared" si="25"/>
@@ -14952,11 +15981,11 @@
       </c>
       <c r="P44">
         <f t="shared" si="25"/>
-        <v>6.833333333333333</v>
+        <v>6.7142857142857144</v>
       </c>
       <c r="Q44">
         <f t="shared" si="25"/>
-        <v>3.5555555555555554</v>
+        <v>3.4</v>
       </c>
       <c r="R44" t="str">
         <f t="shared" si="25"/>
@@ -14966,13 +15995,13 @@
         <f t="shared" si="25"/>
         <v>105.22222222222223</v>
       </c>
-      <c r="T44" t="str">
+      <c r="T44">
         <f t="shared" si="25"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="U44">
         <f t="shared" si="25"/>
-        <v>44.75</v>
+        <v>46.4</v>
       </c>
       <c r="V44">
         <f t="shared" si="25"/>
@@ -14996,7 +16025,7 @@
       </c>
       <c r="AA44">
         <f t="shared" si="25"/>
-        <v>23</v>
+        <v>21.333333333333332</v>
       </c>
       <c r="AB44" t="str">
         <f t="shared" si="25"/>
@@ -15056,7 +16085,7 @@
       </c>
       <c r="AP44">
         <f t="shared" si="25"/>
-        <v>59</v>
+        <v>53.7</v>
       </c>
       <c r="AQ44" t="str">
         <f t="shared" si="25"/>
@@ -15076,7 +16105,7 @@
       </c>
       <c r="AU44">
         <f t="shared" si="25"/>
-        <v>180.5</v>
+        <v>447.28571428571428</v>
       </c>
       <c r="AV44" t="str">
         <f t="shared" si="25"/>
@@ -15107,17 +16136,17 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="3:23">
+    <row r="49" spans="2:23">
       <c r="C49">
         <f>AVERAGE(C44:AA44)</f>
-        <v>23.43398078529658</v>
+        <v>22.925256132756132</v>
       </c>
       <c r="D49">
         <f>AVERAGE(AB44:AZ44)</f>
-        <v>87.409477124183013</v>
+        <v>102.79098972922502</v>
       </c>
     </row>
-    <row r="51" spans="3:23">
+    <row r="51" spans="2:23">
       <c r="C51" t="str">
         <f>C3</f>
         <v>Duration 1000</v>
@@ -15139,29 +16168,29 @@
         <v>Duration 500</v>
       </c>
     </row>
-    <row r="52" spans="3:23">
+    <row r="52" spans="2:23">
       <c r="C52">
         <f>AVERAGE(C44:G44,AB44:AF44)</f>
-        <v>12.638888888888889</v>
+        <v>13.317857142857143</v>
       </c>
       <c r="H52">
         <f>AVERAGE(H44:L44,AG44:AK44)</f>
-        <v>36.323979591836732</v>
+        <v>36.664357864357861</v>
       </c>
       <c r="M52">
         <f>AVERAGE(M44:Q44,AL44:AP44)</f>
-        <v>12.820833333333333</v>
+        <v>12.091053391053391</v>
       </c>
       <c r="R52">
         <f>AVERAGE(R44:V44,AQ44:AU44)</f>
-        <v>140.63425925925927</v>
+        <v>159.7487528344671</v>
       </c>
       <c r="W52">
         <f>AVERAGE(W44:AA44,AV44:AZ44)</f>
-        <v>89.922222222222217</v>
+        <v>89.684126984126991</v>
       </c>
     </row>
-    <row r="55" spans="3:23">
+    <row r="55" spans="2:23">
       <c r="C55" t="str">
         <f>C4</f>
         <v>Amplitude 0</v>
@@ -15183,30 +16212,558 @@
         <v>Amplitude 75</v>
       </c>
     </row>
-    <row r="56" spans="3:23">
+    <row r="56" spans="2:23">
       <c r="C56" t="e">
         <f>AVERAGE(C44,H44,M44,R44,W44,AB44,AG44,AL44,AQ44,AV44)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D56">
         <f>AVERAGE(D44,I44,N44,S44,X44,AC44,AH44,AM44,AR44,AW44)</f>
-        <v>40.105000000000004</v>
+        <v>40.294797979797977</v>
       </c>
       <c r="E56">
         <f>AVERAGE(E44,J44,O44,T44,Y44,AD44,AI44,AN44,AS44,AX44)</f>
-        <v>16.333333333333332</v>
+        <v>14.928571428571429</v>
       </c>
       <c r="F56">
         <f>AVERAGE(F44,K44,P44,U44,Z44,AE44,AJ44,AO44,AT44,AY44)</f>
-        <v>72.539285714285725</v>
+        <v>73.117380952380955</v>
       </c>
       <c r="G56">
         <f>AVERAGE(G44,L44,Q44,V44,AA44,AF44,AK44,AP44,AU44,AZ44)</f>
-        <v>70.676388888888894</v>
+        <v>96.733015873015873</v>
+      </c>
+    </row>
+    <row r="60" spans="2:23">
+      <c r="C60" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61" spans="2:23">
+      <c r="C61" t="str">
+        <f>E55</f>
+        <v>Amplitude 25</v>
+      </c>
+      <c r="D61" t="str">
+        <f>F55</f>
+        <v>Amplitude 50</v>
+      </c>
+      <c r="E61" t="str">
+        <f>G55</f>
+        <v>Amplitude 75</v>
+      </c>
+      <c r="F61" t="str">
+        <f>D55</f>
+        <v>Amplitude 100</v>
+      </c>
+      <c r="I61" t="str">
+        <f>C61</f>
+        <v>Amplitude 25</v>
+      </c>
+      <c r="J61" t="str">
+        <f t="shared" ref="J61:L61" si="26">D61</f>
+        <v>Amplitude 50</v>
+      </c>
+      <c r="K61" t="str">
+        <f t="shared" si="26"/>
+        <v>Amplitude 75</v>
+      </c>
+      <c r="L61" t="str">
+        <f t="shared" si="26"/>
+        <v>Amplitude 100</v>
+      </c>
+    </row>
+    <row r="62" spans="2:23">
+      <c r="B62" t="str">
+        <f>R51</f>
+        <v>Duration 250</v>
+      </c>
+      <c r="D62">
+        <f>U44</f>
+        <v>46.4</v>
+      </c>
+      <c r="E62">
+        <f>V44</f>
+        <v>22.833333333333332</v>
+      </c>
+      <c r="F62">
+        <f>S44</f>
+        <v>105.22222222222223</v>
+      </c>
+      <c r="H62" t="str">
+        <f>B62</f>
+        <v>Duration 250</v>
+      </c>
+      <c r="J62">
+        <f t="shared" ref="J62:L62" si="27">MAX(D62-20,0)</f>
+        <v>26.4</v>
+      </c>
+      <c r="K62">
+        <f t="shared" si="27"/>
+        <v>2.8333333333333321</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="27"/>
+        <v>85.222222222222229</v>
+      </c>
+    </row>
+    <row r="63" spans="2:23">
+      <c r="B63" t="str">
+        <f>W51</f>
+        <v>Duration 500</v>
+      </c>
+      <c r="C63">
+        <f>Y44</f>
+        <v>65</v>
+      </c>
+      <c r="D63">
+        <f>Z44</f>
+        <v>94.4</v>
+      </c>
+      <c r="E63">
+        <f>AA44</f>
+        <v>21.333333333333332</v>
+      </c>
+      <c r="F63">
+        <f>X44</f>
+        <v>15.555555555555555</v>
+      </c>
+      <c r="H63" t="str">
+        <f t="shared" ref="H63:H66" si="28">B63</f>
+        <v>Duration 500</v>
+      </c>
+      <c r="I63">
+        <f t="shared" ref="I63:I66" si="29">MAX(C63-20,0)</f>
+        <v>45</v>
+      </c>
+      <c r="J63">
+        <f t="shared" ref="J63:J66" si="30">MAX(D63-20,0)</f>
+        <v>74.400000000000006</v>
+      </c>
+      <c r="K63">
+        <f t="shared" ref="K63:K66" si="31">MAX(E63-20,0)</f>
+        <v>1.3333333333333321</v>
+      </c>
+      <c r="L63">
+        <f t="shared" ref="L63:L66" si="32">MAX(F63-20,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="2:23">
+      <c r="B64" t="str">
+        <f>C51</f>
+        <v>Duration 1000</v>
+      </c>
+      <c r="C64">
+        <f>E44</f>
+        <v>19</v>
+      </c>
+      <c r="D64">
+        <f>F44</f>
+        <v>7.1428571428571432</v>
+      </c>
+      <c r="E64">
+        <f>G44</f>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="F64">
+        <f>D44</f>
+        <v>7.4</v>
+      </c>
+      <c r="H64" t="str">
+        <f t="shared" si="28"/>
+        <v>Duration 1000</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:12">
+      <c r="B65" t="str">
+        <f>H51</f>
+        <v>Duration 1500</v>
+      </c>
+      <c r="C65">
+        <f>J44</f>
+        <v>5</v>
+      </c>
+      <c r="D65">
+        <f>K44</f>
+        <v>6.25</v>
+      </c>
+      <c r="E65">
+        <f>L44</f>
+        <v>3.7777777777777777</v>
+      </c>
+      <c r="F65">
+        <f>I44</f>
+        <v>4.2727272727272725</v>
+      </c>
+      <c r="H65" t="str">
+        <f t="shared" si="28"/>
+        <v>Duration 1500</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:12">
+      <c r="B66" t="str">
+        <f>M51</f>
+        <v>Duration 2000</v>
+      </c>
+      <c r="C66">
+        <f>O44</f>
+        <v>7.5</v>
+      </c>
+      <c r="D66">
+        <f>P44</f>
+        <v>6.7142857142857144</v>
+      </c>
+      <c r="E66">
+        <f>Q44</f>
+        <v>3.4</v>
+      </c>
+      <c r="F66">
+        <f>N44</f>
+        <v>5.6363636363636367</v>
+      </c>
+      <c r="H66" t="str">
+        <f t="shared" si="28"/>
+        <v>Duration 2000</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:12">
+      <c r="C69" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="70" spans="2:12">
+      <c r="C70" t="str">
+        <f>C61</f>
+        <v>Amplitude 25</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" ref="D70:F70" si="33">D61</f>
+        <v>Amplitude 50</v>
+      </c>
+      <c r="E70" t="str">
+        <f t="shared" si="33"/>
+        <v>Amplitude 75</v>
+      </c>
+      <c r="F70" t="str">
+        <f t="shared" si="33"/>
+        <v>Amplitude 100</v>
+      </c>
+      <c r="I70" t="str">
+        <f>C70</f>
+        <v>Amplitude 25</v>
+      </c>
+      <c r="J70" t="str">
+        <f t="shared" ref="J70" si="34">D70</f>
+        <v>Amplitude 50</v>
+      </c>
+      <c r="K70" t="str">
+        <f t="shared" ref="K70" si="35">E70</f>
+        <v>Amplitude 75</v>
+      </c>
+      <c r="L70" t="str">
+        <f t="shared" ref="L70" si="36">F70</f>
+        <v>Amplitude 100</v>
+      </c>
+    </row>
+    <row r="71" spans="2:12">
+      <c r="B71" t="str">
+        <f>B62</f>
+        <v>Duration 250</v>
+      </c>
+      <c r="D71">
+        <f>AT44</f>
+        <v>385</v>
+      </c>
+      <c r="E71">
+        <f>AU44</f>
+        <v>447.28571428571428</v>
+      </c>
+      <c r="F71">
+        <f>AR44</f>
+        <v>105.5</v>
+      </c>
+      <c r="H71" t="str">
+        <f>B71</f>
+        <v>Duration 250</v>
+      </c>
+      <c r="J71">
+        <f t="shared" ref="J71:J75" si="37">MAX(D71-20,0)</f>
+        <v>365</v>
+      </c>
+      <c r="K71">
+        <f t="shared" ref="K71:K75" si="38">MAX(E71-20,0)</f>
+        <v>427.28571428571428</v>
+      </c>
+      <c r="L71">
+        <f t="shared" ref="L71:L75" si="39">MAX(F71-20,0)</f>
+        <v>85.5</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12">
+      <c r="B72" t="str">
+        <f t="shared" ref="B72:B75" si="40">B63</f>
+        <v>Duration 500</v>
+      </c>
+      <c r="D72">
+        <f>AY44</f>
+        <v>30.666666666666668</v>
+      </c>
+      <c r="E72">
+        <f>AZ44</f>
+        <v>262.83333333333331</v>
+      </c>
+      <c r="F72">
+        <f>AW44</f>
+        <v>138</v>
+      </c>
+      <c r="H72" t="str">
+        <f t="shared" ref="H72:H75" si="41">B72</f>
+        <v>Duration 500</v>
+      </c>
+      <c r="J72">
+        <f t="shared" si="37"/>
+        <v>10.666666666666668</v>
+      </c>
+      <c r="K72">
+        <f t="shared" si="38"/>
+        <v>242.83333333333331</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="39"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="73" spans="2:12">
+      <c r="B73" t="str">
+        <f t="shared" si="40"/>
+        <v>Duration 1000</v>
+      </c>
+      <c r="C73">
+        <f>AD44</f>
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <f>AE44</f>
+        <v>58.333333333333336</v>
+      </c>
+      <c r="E73">
+        <f>AF44</f>
+        <v>4</v>
+      </c>
+      <c r="F73">
+        <f>AC44</f>
+        <v>4</v>
+      </c>
+      <c r="H73" t="str">
+        <f t="shared" si="41"/>
+        <v>Duration 1000</v>
+      </c>
+      <c r="I73">
+        <f t="shared" ref="I73:I75" si="42">MAX(C73-20,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="37"/>
+        <v>38.333333333333336</v>
+      </c>
+      <c r="K73">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="2:12">
+      <c r="B74" t="str">
+        <f t="shared" si="40"/>
+        <v>Duration 1500</v>
+      </c>
+      <c r="D74">
+        <f>AJ44</f>
+        <v>91.6</v>
+      </c>
+      <c r="E74">
+        <f>AK44</f>
+        <v>142.5</v>
+      </c>
+      <c r="F74">
+        <f>AH44</f>
+        <v>3.25</v>
+      </c>
+      <c r="H74" t="str">
+        <f t="shared" si="41"/>
+        <v>Duration 1500</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="37"/>
+        <v>71.599999999999994</v>
+      </c>
+      <c r="K74">
+        <f t="shared" si="38"/>
+        <v>122.5</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="2:12">
+      <c r="B75" t="str">
+        <f t="shared" si="40"/>
+        <v>Duration 2000</v>
+      </c>
+      <c r="C75">
+        <f>AN44</f>
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <f>AO44</f>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="E75">
+        <f>AP44</f>
+        <v>53.7</v>
+      </c>
+      <c r="F75">
+        <f>AM44</f>
+        <v>14.111111111111111</v>
+      </c>
+      <c r="H75" t="str">
+        <f t="shared" si="41"/>
+        <v>Duration 2000</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="J75">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="K75">
+        <f t="shared" si="38"/>
+        <v>33.700000000000003</v>
+      </c>
+      <c r="L75">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:12">
+      <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="J79">
+        <v>150</v>
+      </c>
+      <c r="K79">
+        <v>300</v>
+      </c>
+      <c r="L79">
+        <v>450</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="I62:L66">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I71:L75">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I62:L66 I71:L75 I79:L79">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added small versions of background images.
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="23955" windowHeight="12840"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="23955" windowHeight="12840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="target" sheetId="1" r:id="rId1"/>
     <sheet name="distance" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -372,8 +372,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -901,21 +901,39 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="de-AT"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>target!$C$19:$D$19</c:f>
@@ -946,39 +964,57 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="50737920"/>
-        <c:axId val="50739456"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="103979520"/>
+        <c:axId val="14099584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50737920"/>
+        <c:axId val="103979520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50739456"/>
+        <c:crossAx val="14099584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50739456"/>
+        <c:axId val="14099584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50737920"/>
+        <c:crossAx val="103979520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -990,16 +1026,29 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="de-AT"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>(target!$C$22,target!$H$22,target!$M$22,target!$R$22,target!$W$22)</c:f>
@@ -1048,39 +1097,57 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="50758784"/>
-        <c:axId val="50760320"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="81894400"/>
+        <c:axId val="14101312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50758784"/>
+        <c:axId val="81894400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50760320"/>
+        <c:crossAx val="14101312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50760320"/>
+        <c:axId val="14101312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50758784"/>
+        <c:crossAx val="81894400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1092,16 +1159,29 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="de-AT"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>target!$C$25:$G$25</c:f>
@@ -1150,37 +1230,55 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="51254784"/>
-        <c:axId val="51256320"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="83461120"/>
+        <c:axId val="14104192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="51254784"/>
+        <c:axId val="83461120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51256320"/>
+        <c:crossAx val="14104192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51256320"/>
+        <c:axId val="14104192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51254784"/>
+        <c:crossAx val="83461120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1192,16 +1290,29 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="de-AT"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>target!$C$5:$AZ$5</c:f>
@@ -1520,39 +1631,57 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="51296128"/>
-        <c:axId val="51297664"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="103991296"/>
+        <c:axId val="61293696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="51296128"/>
+        <c:axId val="103991296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51297664"/>
+        <c:crossAx val="61293696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51297664"/>
+        <c:axId val="61293696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51296128"/>
+        <c:crossAx val="103991296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1564,16 +1693,29 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="de-AT"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>target!$C$29:$D$29</c:f>
@@ -1604,39 +1746,57 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="51190016"/>
-        <c:axId val="51200000"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="103991808"/>
+        <c:axId val="61296000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="51190016"/>
+        <c:axId val="103991808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51200000"/>
+        <c:crossAx val="61296000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51200000"/>
+        <c:axId val="61296000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51190016"/>
+        <c:crossAx val="103991808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1648,16 +1808,29 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="de-AT"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>distance!$C$48:$D$48</c:f>
@@ -1688,37 +1861,55 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="51338240"/>
-        <c:axId val="51340032"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="103992832"/>
+        <c:axId val="61298304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="51338240"/>
+        <c:axId val="103992832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51340032"/>
+        <c:crossAx val="61298304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51340032"/>
+        <c:axId val="61298304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51338240"/>
+        <c:crossAx val="103992832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1730,16 +1921,29 @@
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="de-AT"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>(distance!$C$51,distance!$H$51,distance!$M$51,distance!$R$51,distance!$W$51)</c:f>
@@ -1788,37 +1992,55 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="51355008"/>
-        <c:axId val="51364992"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="61886464"/>
+        <c:axId val="61300032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="51355008"/>
+        <c:axId val="61886464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51364992"/>
+        <c:crossAx val="61300032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51364992"/>
+        <c:axId val="61300032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51355008"/>
+        <c:crossAx val="61886464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1830,16 +2052,29 @@
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="de-AT"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>distance!$C$55:$G$55</c:f>
@@ -1888,37 +2123,55 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="50355584"/>
-        <c:axId val="51471488"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="123318784"/>
+        <c:axId val="96292800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50355584"/>
+        <c:axId val="123318784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51471488"/>
+        <c:crossAx val="96292800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51471488"/>
+        <c:axId val="96292800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50355584"/>
+        <c:crossAx val="123318784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2087,16 +2340,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1879890</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>19916</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>791319</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>74345</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>1472047</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>96116</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>437905</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>150545</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2253,6 +2506,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2287,6 +2541,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2462,14 +2717,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DA55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:DA57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AI56" sqref="AI56"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="37.42578125" customWidth="1"/>
@@ -2477,7 +2732,7 @@
     <col min="5" max="5" width="36.7109375" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
     <col min="7" max="7" width="38" customWidth="1"/>
-    <col min="8" max="8" width="52.140625" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" customWidth="1"/>
     <col min="10" max="10" width="27.140625" customWidth="1"/>
     <col min="11" max="12" width="12.7109375" customWidth="1"/>
@@ -2493,7 +2748,7 @@
     <col min="54" max="102" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:105">
+    <row r="1" spans="1:105" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>26</v>
       </c>
@@ -2893,7 +3148,7 @@
         <v>Repetition 2</v>
       </c>
     </row>
-    <row r="2" spans="1:105">
+    <row r="2" spans="1:105" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>28</v>
       </c>
@@ -3293,7 +3548,7 @@
         <v>Peripheral</v>
       </c>
     </row>
-    <row r="3" spans="1:105">
+    <row r="3" spans="1:105" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>33</v>
       </c>
@@ -3690,7 +3945,7 @@
         <v>Duration 500</v>
       </c>
     </row>
-    <row r="4" spans="1:105">
+    <row r="4" spans="1:105" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>30</v>
       </c>
@@ -4087,7 +4342,7 @@
         <v>Amplitude 75</v>
       </c>
     </row>
-    <row r="5" spans="1:105">
+    <row r="5" spans="1:105" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -4395,7 +4650,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:105">
+    <row r="6" spans="1:105" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4704,7 +4959,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:105">
+    <row r="7" spans="1:105" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -5013,7 +5268,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:105">
+    <row r="8" spans="1:105" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -5322,7 +5577,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:105">
+    <row r="9" spans="1:105" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -5631,7 +5886,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:105">
+    <row r="10" spans="1:105" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -5940,7 +6195,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:105">
+    <row r="11" spans="1:105" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -6249,12 +6504,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:105">
+    <row r="16" spans="1:105" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="3:52">
+    <row r="17" spans="3:52" x14ac:dyDescent="0.25">
       <c r="C17">
         <f>AVERAGE(C6:C14,BA6:BA15)</f>
         <v>0</v>
@@ -6456,7 +6711,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="3:52">
+    <row r="19" spans="3:52" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>28</v>
       </c>
@@ -6464,7 +6719,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="3:52">
+    <row r="20" spans="3:52" x14ac:dyDescent="0.25">
       <c r="C20">
         <f>AVERAGE(C17:AA17)</f>
         <v>0.4933333333333334</v>
@@ -6474,7 +6729,7 @@
         <v>0.30333333333333334</v>
       </c>
     </row>
-    <row r="22" spans="3:52">
+    <row r="22" spans="3:52" x14ac:dyDescent="0.25">
       <c r="C22" t="str">
         <f>C3</f>
         <v>Duration 1000</v>
@@ -6496,7 +6751,7 @@
         <v>Duration 500</v>
       </c>
     </row>
-    <row r="23" spans="3:52">
+    <row r="23" spans="3:52" x14ac:dyDescent="0.25">
       <c r="C23">
         <f>AVERAGE(C17:G17,AB17:AF17)</f>
         <v>0.39166666666666672</v>
@@ -6518,7 +6773,7 @@
         <v>0.38333333333333336</v>
       </c>
     </row>
-    <row r="25" spans="3:52">
+    <row r="25" spans="3:52" x14ac:dyDescent="0.25">
       <c r="C25" t="str">
         <f>C4</f>
         <v>Amplitude 0</v>
@@ -6540,7 +6795,7 @@
         <v>Amplitude 75</v>
       </c>
     </row>
-    <row r="26" spans="3:52">
+    <row r="26" spans="3:52" x14ac:dyDescent="0.25">
       <c r="C26">
         <f>AVERAGE(C17,H17,M17,R17,W17,AB17,AG17,AL17,AQ17,AV17)</f>
         <v>8.3333333333333332E-3</v>
@@ -6562,7 +6817,7 @@
         <v>0.64166666666666661</v>
       </c>
     </row>
-    <row r="29" spans="3:52">
+    <row r="29" spans="3:52" x14ac:dyDescent="0.25">
       <c r="C29" t="str">
         <f>C1</f>
         <v>Repetition 1</v>
@@ -6572,7 +6827,7 @@
         <v>Repetition 2</v>
       </c>
     </row>
-    <row r="30" spans="3:52">
+    <row r="30" spans="3:52" x14ac:dyDescent="0.25">
       <c r="C30">
         <f>AVERAGE(C6:AZ6)</f>
         <v>0.54</v>
@@ -6582,12 +6837,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" spans="2:7">
-      <c r="C34" t="s">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C34" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:7">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C35" t="str">
         <f>C25</f>
         <v>Amplitude 0</v>
@@ -6609,7 +6864,7 @@
         <v>Amplitude 100</v>
       </c>
     </row>
-    <row r="36" spans="2:7">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>R22</f>
         <v>Duration 250</v>
@@ -6634,8 +6889,12 @@
         <f>S17</f>
         <v>0.83333333333333337</v>
       </c>
+      <c r="I36">
+        <f>AVERAGE(C36:G36)</f>
+        <v>0.3666666666666667</v>
+      </c>
     </row>
-    <row r="37" spans="2:7">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>W22</f>
         <v>Duration 500</v>
@@ -6660,8 +6919,12 @@
         <f>X17</f>
         <v>0.83333333333333337</v>
       </c>
+      <c r="I37">
+        <f t="shared" ref="I37:I54" si="17">AVERAGE(C37:G37)</f>
+        <v>0.48333333333333328</v>
+      </c>
     </row>
-    <row r="38" spans="2:7">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f>C22</f>
         <v>Duration 1000</v>
@@ -6686,8 +6949,12 @@
         <f>D17</f>
         <v>0.83333333333333337</v>
       </c>
+      <c r="I38">
+        <f t="shared" si="17"/>
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="39" spans="2:7">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>H22</f>
         <v>Duration 1500</v>
@@ -6712,8 +6979,12 @@
         <f>I17</f>
         <v>1</v>
       </c>
+      <c r="I39">
+        <f t="shared" si="17"/>
+        <v>0.55000000000000004</v>
+      </c>
     </row>
-    <row r="40" spans="2:7">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>M22</f>
         <v>Duration 2000</v>
@@ -6738,35 +7009,65 @@
         <f>N17</f>
         <v>1</v>
       </c>
+      <c r="I40">
+        <f t="shared" si="17"/>
+        <v>0.56666666666666665</v>
+      </c>
     </row>
-    <row r="46" spans="2:7">
-      <c r="C46" t="s">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <f>AVERAGE(C36:C40)</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="D42">
+        <f t="shared" ref="D42:G42" si="18">AVERAGE(D36:D40)</f>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="18"/>
+        <v>0.6</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="18"/>
+        <v>0.75</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="18"/>
+        <v>0.9</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="17"/>
+        <v>0.49333333333333335</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C46" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="2:7">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C47" t="str">
         <f>C35</f>
         <v>Amplitude 0</v>
       </c>
       <c r="D47" t="str">
-        <f t="shared" ref="D47:G47" si="17">D35</f>
+        <f t="shared" ref="D47:G47" si="19">D35</f>
         <v>Amplitude 25</v>
       </c>
       <c r="E47" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>Amplitude 50</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>Amplitude 75</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>Amplitude 100</v>
       </c>
     </row>
-    <row r="48" spans="2:7">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" t="str">
         <f>B36</f>
         <v>Duration 250</v>
@@ -6791,10 +7092,14 @@
         <f>AR17</f>
         <v>0.16666666666666666</v>
       </c>
+      <c r="I48">
+        <f t="shared" si="17"/>
+        <v>0.16666666666666669</v>
+      </c>
     </row>
-    <row r="49" spans="2:7">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" t="str">
-        <f t="shared" ref="B49:B52" si="18">B37</f>
+        <f t="shared" ref="B49:B52" si="20">B37</f>
         <v>Duration 500</v>
       </c>
       <c r="C49">
@@ -6817,10 +7122,14 @@
         <f>AW17</f>
         <v>0.66666666666666663</v>
       </c>
+      <c r="I49">
+        <f t="shared" si="17"/>
+        <v>0.28333333333333333</v>
+      </c>
     </row>
-    <row r="50" spans="2:7">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>Duration 1000</v>
       </c>
       <c r="C50">
@@ -6843,10 +7152,14 @@
         <f>AC17</f>
         <v>0.66666666666666663</v>
       </c>
+      <c r="I50">
+        <f t="shared" si="17"/>
+        <v>0.28333333333333333</v>
+      </c>
     </row>
-    <row r="51" spans="2:7">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>Duration 1500</v>
       </c>
       <c r="C51">
@@ -6869,10 +7182,14 @@
         <f>AH17</f>
         <v>0.66666666666666663</v>
       </c>
+      <c r="I51">
+        <f t="shared" si="17"/>
+        <v>0.33333333333333331</v>
+      </c>
     </row>
-    <row r="52" spans="2:7">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>Duration 2000</v>
       </c>
       <c r="C52">
@@ -6895,43 +7212,85 @@
         <f>AM17</f>
         <v>0.75</v>
       </c>
+      <c r="I52">
+        <f t="shared" si="17"/>
+        <v>0.45</v>
+      </c>
     </row>
-    <row r="55" spans="2:7">
-      <c r="C55">
-        <v>0</v>
-      </c>
-      <c r="D55">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <f>AVERAGE(C48:C52)</f>
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <f t="shared" ref="D54:F54" si="21">AVERAGE(D48:D52)</f>
+        <v>0.05</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="21"/>
+        <v>0.35</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="21"/>
+        <v>0.53333333333333344</v>
+      </c>
+      <c r="G54">
+        <f>AVERAGE(G48:G52)</f>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="17"/>
+        <v>0.30333333333333334</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
         <v>0.25</v>
       </c>
-      <c r="E55">
+      <c r="E57">
         <v>0.5</v>
       </c>
-      <c r="F55">
+      <c r="F57">
         <v>0.75</v>
       </c>
-      <c r="G55">
+      <c r="G57">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C36:G40">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C48:G52 C55:G55">
+  <conditionalFormatting sqref="C57:G57 C48:G52">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36:G40 I36:I40 I42 C42:G42 C48:G52 C54:G54 I48:I52 I54 C57:G57">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6945,14 +7304,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CX79"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M86" sqref="M86"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N86" sqref="N86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -7015,7 +7374,7 @@
     <col min="100" max="102" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:102">
+    <row r="1" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>target!A1</f>
         <v>0</v>
@@ -7425,7 +7784,7 @@
         <v>Repetition 2</v>
       </c>
     </row>
-    <row r="2" spans="1:102">
+    <row r="2" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>target!A2</f>
         <v>0</v>
@@ -7835,7 +8194,7 @@
         <v>Peripheral</v>
       </c>
     </row>
-    <row r="3" spans="1:102">
+    <row r="3" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>target!A3</f>
         <v>0</v>
@@ -8245,7 +8604,7 @@
         <v>Duration 500</v>
       </c>
     </row>
-    <row r="4" spans="1:102">
+    <row r="4" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>target!A4</f>
         <v>0</v>
@@ -8655,7 +9014,7 @@
         <v>Amplitude 75</v>
       </c>
     </row>
-    <row r="5" spans="1:102">
+    <row r="5" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>target!A5</f>
         <v>userID</v>
@@ -9065,7 +9424,7 @@
         <v>rep_1--ecc_1--dur_500--amp_75</v>
       </c>
     </row>
-    <row r="6" spans="1:102">
+    <row r="6" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -9370,7 +9729,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:102">
+    <row r="7" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -9675,7 +10034,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="8" spans="1:102">
+    <row r="8" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -9980,7 +10339,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:102">
+    <row r="9" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -10285,7 +10644,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:102">
+    <row r="10" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -10590,7 +10949,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:102">
+    <row r="11" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -10895,7 +11254,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="3:102">
+    <row r="22" spans="3:102" x14ac:dyDescent="0.25">
       <c r="C22" t="str">
         <f>IF(C6&gt;=0,C6,"")</f>
         <v/>
@@ -11297,7 +11656,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="3:102">
+    <row r="23" spans="3:102" x14ac:dyDescent="0.25">
       <c r="C23" t="str">
         <f t="shared" ref="C23:BN23" si="2">IF(C7&gt;=0,C7,"")</f>
         <v/>
@@ -11699,7 +12058,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="24" spans="3:102">
+    <row r="24" spans="3:102" x14ac:dyDescent="0.25">
       <c r="C24" t="str">
         <f t="shared" ref="C24:BN24" si="4">IF(C8&gt;=0,C8,"")</f>
         <v/>
@@ -12101,7 +12460,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="3:102">
+    <row r="25" spans="3:102" x14ac:dyDescent="0.25">
       <c r="C25" t="str">
         <f t="shared" ref="C25:BN25" si="6">IF(C9&gt;=0,C9,"")</f>
         <v/>
@@ -12503,7 +12862,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="3:102">
+    <row r="26" spans="3:102" x14ac:dyDescent="0.25">
       <c r="C26" t="str">
         <f t="shared" ref="C26:BN26" si="8">IF(C10&gt;=0,C10,"")</f>
         <v/>
@@ -12905,7 +13264,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="3:102">
+    <row r="27" spans="3:102" x14ac:dyDescent="0.25">
       <c r="C27" t="str">
         <f t="shared" ref="C27:BN27" si="10">IF(C11&gt;=0,C11,"")</f>
         <v/>
@@ -13307,7 +13666,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="3:102">
+    <row r="28" spans="3:102" x14ac:dyDescent="0.25">
       <c r="C28">
         <f t="shared" ref="C28:BN28" si="12">IF(C12&gt;=0,C12,"")</f>
         <v>0</v>
@@ -13709,7 +14068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="3:102">
+    <row r="29" spans="3:102" x14ac:dyDescent="0.25">
       <c r="C29">
         <f t="shared" ref="C29:BN29" si="14">IF(C13&gt;=0,C13,"")</f>
         <v>0</v>
@@ -14111,7 +14470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="3:102">
+    <row r="30" spans="3:102" x14ac:dyDescent="0.25">
       <c r="C30">
         <f t="shared" ref="C30:BN30" si="16">IF(C14&gt;=0,C14,"")</f>
         <v>0</v>
@@ -14513,7 +14872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="3:102">
+    <row r="31" spans="3:102" x14ac:dyDescent="0.25">
       <c r="C31">
         <f t="shared" ref="C31:BN31" si="18">IF(C15&gt;=0,C15,"")</f>
         <v>0</v>
@@ -14915,7 +15274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="3:102">
+    <row r="32" spans="3:102" x14ac:dyDescent="0.25">
       <c r="C32">
         <f t="shared" ref="C32:BN32" si="20">IF(C16&gt;=0,C16,"")</f>
         <v>0</v>
@@ -15317,7 +15676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:102">
+    <row r="33" spans="3:102" x14ac:dyDescent="0.25">
       <c r="C33">
         <f t="shared" ref="C33:BN33" si="22">IF(C17&gt;=0,C17,"")</f>
         <v>0</v>
@@ -15719,12 +16078,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="3:102">
+    <row r="42" spans="3:102" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="3:102">
+    <row r="43" spans="3:102" x14ac:dyDescent="0.25">
       <c r="C43" t="e">
         <f>AVERAGE(C22:C27,BA22:BA26)</f>
         <v>#DIV/0!</v>
@@ -15926,7 +16285,7 @@
         <v>262.83333333333331</v>
       </c>
     </row>
-    <row r="44" spans="3:102">
+    <row r="44" spans="3:102" x14ac:dyDescent="0.25">
       <c r="C44" t="str">
         <f>IF(ISNUMBER(C43),C43,"")</f>
         <v/>
@@ -16128,7 +16487,7 @@
         <v>262.83333333333331</v>
       </c>
     </row>
-    <row r="48" spans="3:102">
+    <row r="48" spans="3:102" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>28</v>
       </c>
@@ -16136,7 +16495,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="2:23">
+    <row r="49" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C49">
         <f>AVERAGE(C44:AA44)</f>
         <v>22.925256132756132</v>
@@ -16146,7 +16505,7 @@
         <v>102.79098972922502</v>
       </c>
     </row>
-    <row r="51" spans="2:23">
+    <row r="51" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C51" t="str">
         <f>C3</f>
         <v>Duration 1000</v>
@@ -16168,7 +16527,7 @@
         <v>Duration 500</v>
       </c>
     </row>
-    <row r="52" spans="2:23">
+    <row r="52" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C52">
         <f>AVERAGE(C44:G44,AB44:AF44)</f>
         <v>13.317857142857143</v>
@@ -16190,7 +16549,7 @@
         <v>89.684126984126991</v>
       </c>
     </row>
-    <row r="55" spans="2:23">
+    <row r="55" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C55" t="str">
         <f>C4</f>
         <v>Amplitude 0</v>
@@ -16212,7 +16571,7 @@
         <v>Amplitude 75</v>
       </c>
     </row>
-    <row r="56" spans="2:23">
+    <row r="56" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C56" t="e">
         <f>AVERAGE(C44,H44,M44,R44,W44,AB44,AG44,AL44,AQ44,AV44)</f>
         <v>#DIV/0!</v>
@@ -16234,12 +16593,12 @@
         <v>96.733015873015873</v>
       </c>
     </row>
-    <row r="60" spans="2:23">
+    <row r="60" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="2:23">
+    <row r="61" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C61" t="str">
         <f>E55</f>
         <v>Amplitude 25</v>
@@ -16273,7 +16632,7 @@
         <v>Amplitude 100</v>
       </c>
     </row>
-    <row r="62" spans="2:23">
+    <row r="62" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B62" t="str">
         <f>R51</f>
         <v>Duration 250</v>
@@ -16306,8 +16665,12 @@
         <f t="shared" si="27"/>
         <v>85.222222222222229</v>
       </c>
+      <c r="N62">
+        <f>AVERAGE(I62:L62)</f>
+        <v>38.151851851851852</v>
+      </c>
     </row>
-    <row r="63" spans="2:23">
+    <row r="63" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B63" t="str">
         <f>W51</f>
         <v>Duration 500</v>
@@ -16348,8 +16711,12 @@
         <f t="shared" ref="L63:L66" si="32">MAX(F63-20,0)</f>
         <v>0</v>
       </c>
+      <c r="N63">
+        <f t="shared" ref="N63:N67" si="33">AVERAGE(I63:L63)</f>
+        <v>30.183333333333334</v>
+      </c>
     </row>
-    <row r="64" spans="2:23">
+    <row r="64" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B64" t="str">
         <f>C51</f>
         <v>Duration 1000</v>
@@ -16390,8 +16757,12 @@
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
+      <c r="N64">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="65" spans="2:12">
+    <row r="65" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B65" t="str">
         <f>H51</f>
         <v>Duration 1500</v>
@@ -16432,8 +16803,12 @@
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
+      <c r="N65">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="2:12">
+    <row r="66" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B66" t="str">
         <f>M51</f>
         <v>Duration 2000</v>
@@ -16474,27 +16849,31 @@
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
+      <c r="N66">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="2:12">
+    <row r="69" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="2:12">
+    <row r="70" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C70" t="str">
         <f>C61</f>
         <v>Amplitude 25</v>
       </c>
       <c r="D70" t="str">
-        <f t="shared" ref="D70:F70" si="33">D61</f>
+        <f t="shared" ref="D70:F70" si="34">D61</f>
         <v>Amplitude 50</v>
       </c>
       <c r="E70" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>Amplitude 75</v>
       </c>
       <c r="F70" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>Amplitude 100</v>
       </c>
       <c r="I70" t="str">
@@ -16502,19 +16881,19 @@
         <v>Amplitude 25</v>
       </c>
       <c r="J70" t="str">
-        <f t="shared" ref="J70" si="34">D70</f>
+        <f t="shared" ref="J70" si="35">D70</f>
         <v>Amplitude 50</v>
       </c>
       <c r="K70" t="str">
-        <f t="shared" ref="K70" si="35">E70</f>
+        <f t="shared" ref="K70" si="36">E70</f>
         <v>Amplitude 75</v>
       </c>
       <c r="L70" t="str">
-        <f t="shared" ref="L70" si="36">F70</f>
+        <f t="shared" ref="L70" si="37">F70</f>
         <v>Amplitude 100</v>
       </c>
     </row>
-    <row r="71" spans="2:12">
+    <row r="71" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B71" t="str">
         <f>B62</f>
         <v>Duration 250</v>
@@ -16536,21 +16915,25 @@
         <v>Duration 250</v>
       </c>
       <c r="J71">
-        <f t="shared" ref="J71:J75" si="37">MAX(D71-20,0)</f>
+        <f t="shared" ref="J71:J75" si="38">MAX(D71-20,0)</f>
         <v>365</v>
       </c>
       <c r="K71">
-        <f t="shared" ref="K71:K75" si="38">MAX(E71-20,0)</f>
+        <f t="shared" ref="K71:K75" si="39">MAX(E71-20,0)</f>
         <v>427.28571428571428</v>
       </c>
       <c r="L71">
-        <f t="shared" ref="L71:L75" si="39">MAX(F71-20,0)</f>
+        <f t="shared" ref="L71:L75" si="40">MAX(F71-20,0)</f>
         <v>85.5</v>
       </c>
+      <c r="N71">
+        <f>AVERAGE(I71:L71)</f>
+        <v>292.59523809523807</v>
+      </c>
     </row>
-    <row r="72" spans="2:12">
+    <row r="72" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B72" t="str">
-        <f t="shared" ref="B72:B75" si="40">B63</f>
+        <f t="shared" ref="B72:B75" si="41">B63</f>
         <v>Duration 500</v>
       </c>
       <c r="D72">
@@ -16566,25 +16949,29 @@
         <v>138</v>
       </c>
       <c r="H72" t="str">
-        <f t="shared" ref="H72:H75" si="41">B72</f>
+        <f t="shared" ref="H72:H75" si="42">B72</f>
         <v>Duration 500</v>
       </c>
       <c r="J72">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>10.666666666666668</v>
       </c>
       <c r="K72">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>242.83333333333331</v>
       </c>
       <c r="L72">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>118</v>
       </c>
+      <c r="N72">
+        <f t="shared" ref="N72:N75" si="43">AVERAGE(I72:L72)</f>
+        <v>123.83333333333333</v>
+      </c>
     </row>
-    <row r="73" spans="2:12">
+    <row r="73" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B73" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>Duration 1000</v>
       </c>
       <c r="C73">
@@ -16604,29 +16991,33 @@
         <v>4</v>
       </c>
       <c r="H73" t="str">
+        <f t="shared" si="42"/>
+        <v>Duration 1000</v>
+      </c>
+      <c r="I73">
+        <f t="shared" ref="I73:I75" si="44">MAX(C73-20,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="38"/>
+        <v>38.333333333333336</v>
+      </c>
+      <c r="K73">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="N73">
+        <f t="shared" si="43"/>
+        <v>9.5833333333333339</v>
+      </c>
+    </row>
+    <row r="74" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B74" t="str">
         <f t="shared" si="41"/>
-        <v>Duration 1000</v>
-      </c>
-      <c r="I73">
-        <f t="shared" ref="I73:I75" si="42">MAX(C73-20,0)</f>
-        <v>0</v>
-      </c>
-      <c r="J73">
-        <f t="shared" si="37"/>
-        <v>38.333333333333336</v>
-      </c>
-      <c r="K73">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="L73">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="2:12">
-      <c r="B74" t="str">
-        <f t="shared" si="40"/>
         <v>Duration 1500</v>
       </c>
       <c r="D74">
@@ -16642,25 +17033,29 @@
         <v>3.25</v>
       </c>
       <c r="H74" t="str">
+        <f t="shared" si="42"/>
+        <v>Duration 1500</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="38"/>
+        <v>71.599999999999994</v>
+      </c>
+      <c r="K74">
+        <f t="shared" si="39"/>
+        <v>122.5</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="N74">
+        <f t="shared" si="43"/>
+        <v>64.7</v>
+      </c>
+    </row>
+    <row r="75" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B75" t="str">
         <f t="shared" si="41"/>
-        <v>Duration 1500</v>
-      </c>
-      <c r="J74">
-        <f t="shared" si="37"/>
-        <v>71.599999999999994</v>
-      </c>
-      <c r="K74">
-        <f t="shared" si="38"/>
-        <v>122.5</v>
-      </c>
-      <c r="L74">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="2:12">
-      <c r="B75" t="str">
-        <f t="shared" si="40"/>
         <v>Duration 2000</v>
       </c>
       <c r="C75">
@@ -16680,27 +17075,31 @@
         <v>14.111111111111111</v>
       </c>
       <c r="H75" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>Duration 2000</v>
       </c>
       <c r="I75">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="J75">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="K75">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>33.700000000000003</v>
       </c>
       <c r="L75">
-        <f t="shared" si="39"/>
-        <v>0</v>
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="N75">
+        <f t="shared" si="43"/>
+        <v>8.4250000000000007</v>
       </c>
     </row>
-    <row r="79" spans="2:12">
+    <row r="79" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I79">
         <v>0</v>
       </c>
@@ -16718,9 +17117,9 @@
   <conditionalFormatting sqref="I62:L66">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -16730,9 +17129,9 @@
   <conditionalFormatting sqref="I71:L75">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -16742,9 +17141,9 @@
   <conditionalFormatting sqref="I62:L66 I71:L75 I79:L79">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -16757,12 +17156,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Pilot 1: results updated.
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="23955" windowHeight="12840" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="23955" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="target" sheetId="1" r:id="rId1"/>
@@ -8649,8 +8649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DI93"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J59" sqref="J59"/>
+    <sheetView tabSelected="1" topLeftCell="J12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AB80" sqref="AB80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50643,7 +50643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DG156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A111" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D154" sqref="D154"/>
     </sheetView>
   </sheetViews>

</xml_diff>